<commit_message>
Part number tweaks for v0.4.3 board
</commit_message>
<xml_diff>
--- a/reference/hardware/v0.4/BOMs/v0.4.3_bom.xlsx
+++ b/reference/hardware/v0.4/BOMs/v0.4.3_bom.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="27815"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="28109"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/josh/Documents/Arduino/speeduino/reference/hardware/v0.4/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/josh/Documents/Arduino/speeduino/reference/hardware/v0.4/BOMs/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -507,9 +507,6 @@
     <t>R11,14,35,37,48,49,55,56</t>
   </si>
   <si>
-    <t>R9,12,26,28</t>
-  </si>
-  <si>
     <t>C11,20</t>
   </si>
   <si>
@@ -813,9 +810,6 @@
     <t>Q1,Q2,Q3,Q4,Q5,Q6,Q7,Q8</t>
   </si>
   <si>
-    <t>R9,R12,R15,R18,R26,R28,R33,R34</t>
-  </si>
-  <si>
     <t>R2,R4,R6,R8,R22,R41</t>
   </si>
   <si>
@@ -855,12 +849,6 @@
     <t>603-MFR-25FBF52-2K49</t>
   </si>
   <si>
-    <t>R1,R3,R61</t>
-  </si>
-  <si>
-    <t>R1,3,R61</t>
-  </si>
-  <si>
     <t>C19,C25</t>
   </si>
   <si>
@@ -877,6 +865,18 @@
   </si>
   <si>
     <t>R10,13,R21,23,24,R39,R40,50,51,57,58,59,60</t>
+  </si>
+  <si>
+    <t>R9,R12,R15,R18</t>
+  </si>
+  <si>
+    <t>R1,R3,R26,R28,R33,R34,R61</t>
+  </si>
+  <si>
+    <t>R9,12</t>
+  </si>
+  <si>
+    <t>R1,3,R26,R28,R61</t>
   </si>
 </sst>
 </file>
@@ -1600,8 +1600,8 @@
   </sheetPr>
   <dimension ref="A1:Z46"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="138" workbookViewId="0">
+      <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1623,16 +1623,16 @@
   <sheetData>
     <row r="1" spans="1:26" ht="27" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="16" t="s">
+        <v>169</v>
+      </c>
+      <c r="B1" s="16" t="s">
         <v>170</v>
       </c>
-      <c r="B1" s="16" t="s">
+      <c r="C1" s="1" t="s">
         <v>171</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>172</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>173</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>0</v>
@@ -1653,7 +1653,7 @@
         <v>4</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="L1" s="1" t="s">
         <v>5</v>
@@ -1662,40 +1662,40 @@
         <v>6</v>
       </c>
       <c r="N1" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="O1" s="1" t="s">
         <v>189</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>190</v>
       </c>
-      <c r="P1" s="1" t="s">
-        <v>191</v>
-      </c>
       <c r="Q1" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="R1" s="1" t="s">
         <v>218</v>
       </c>
-      <c r="R1" s="1" t="s">
-        <v>219</v>
-      </c>
       <c r="S1" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="T1" s="1" t="s">
         <v>226</v>
-      </c>
-      <c r="T1" s="1" t="s">
-        <v>227</v>
       </c>
       <c r="U1" s="1" t="s">
         <v>7</v>
       </c>
       <c r="V1" s="20" t="s">
+        <v>185</v>
+      </c>
+      <c r="W1" s="20" t="s">
         <v>186</v>
-      </c>
-      <c r="W1" s="20" t="s">
-        <v>187</v>
       </c>
       <c r="X1" s="20" t="s">
         <v>125</v>
       </c>
       <c r="Y1" s="20" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="2" spans="1:26" ht="17" thickBot="1" x14ac:dyDescent="0.25">
@@ -1752,7 +1752,7 @@
         <v>8</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="G3" s="3" t="s">
         <v>9</v>
@@ -1765,16 +1765,16 @@
         <v>13</v>
       </c>
       <c r="K3" s="3" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="L3" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="M3" s="2" t="s">
         <v>155</v>
       </c>
-      <c r="M3" s="2" t="s">
-        <v>156</v>
-      </c>
       <c r="N3" s="2" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="O3" s="5">
         <v>1.7</v>
@@ -1830,16 +1830,16 @@
         <v>6</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>260</v>
+        <v>256</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
       <c r="E4" s="3" t="s">
         <v>11</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="G4" s="3" t="s">
         <v>12</v>
@@ -1852,16 +1852,16 @@
         <v>13</v>
       </c>
       <c r="K4" s="3" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="L4" s="3" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="M4" s="2" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="N4" s="2" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="O4" s="5">
         <v>0.66</v>
@@ -1917,7 +1917,7 @@
         <v>7</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="D5" s="4" t="s">
         <v>89</v>
@@ -1926,7 +1926,7 @@
         <v>14</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="G5" s="3" t="s">
         <v>12</v>
@@ -1939,16 +1939,16 @@
         <v>13</v>
       </c>
       <c r="K5" s="3" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="L5" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="M5" s="2" t="s">
         <v>149</v>
       </c>
-      <c r="M5" s="2" t="s">
-        <v>150</v>
-      </c>
       <c r="N5" s="2" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="O5" s="5">
         <v>0.32</v>
@@ -2013,7 +2013,7 @@
         <v>15</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="G6" s="3" t="s">
         <v>9</v>
@@ -2026,16 +2026,16 @@
         <v>13</v>
       </c>
       <c r="K6" s="3" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="L6" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="M6" s="2" t="s">
         <v>158</v>
       </c>
-      <c r="M6" s="2" t="s">
-        <v>159</v>
-      </c>
       <c r="N6" s="2" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="O6" s="5">
         <v>1.57</v>
@@ -2100,7 +2100,7 @@
         <v>16</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="G7" s="3" t="s">
         <v>12</v>
@@ -2113,16 +2113,16 @@
         <v>10</v>
       </c>
       <c r="K7" s="3" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="L7" s="3" t="s">
+        <v>159</v>
+      </c>
+      <c r="M7" s="2" t="s">
         <v>160</v>
       </c>
-      <c r="M7" s="2" t="s">
-        <v>161</v>
-      </c>
       <c r="N7" s="2" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="O7" s="5">
         <v>0.62</v>
@@ -2178,16 +2178,16 @@
         <v>2</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
       <c r="E8" s="3" t="s">
         <v>17</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="G8" s="3" t="s">
         <v>12</v>
@@ -2200,16 +2200,16 @@
         <v>13</v>
       </c>
       <c r="K8" s="3" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="L8" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="M8" s="2" t="s">
         <v>164</v>
       </c>
-      <c r="M8" s="2" t="s">
-        <v>165</v>
-      </c>
       <c r="N8" s="2" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="O8" s="5">
         <v>0.24</v>
@@ -2265,16 +2265,16 @@
         <v>2</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="D9" s="23" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E9" s="3" t="s">
         <v>18</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="G9" s="3" t="s">
         <v>12</v>
@@ -2287,16 +2287,16 @@
         <v>13</v>
       </c>
       <c r="K9" s="3" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="L9" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="M9" s="2" t="s">
         <v>146</v>
       </c>
-      <c r="M9" s="2" t="s">
-        <v>147</v>
-      </c>
       <c r="N9" s="2" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="O9" s="5">
         <v>0.66</v>
@@ -2372,7 +2372,7 @@
         <v>13</v>
       </c>
       <c r="K10" s="3" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="L10" s="3" t="s">
         <v>118</v>
@@ -2381,7 +2381,7 @@
         <v>117</v>
       </c>
       <c r="N10" s="2" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="O10" s="5">
         <v>0.25</v>
@@ -2498,7 +2498,7 @@
         <v>21</v>
       </c>
       <c r="K12" s="3" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="L12" s="7" t="s">
         <v>22</v>
@@ -2507,7 +2507,7 @@
         <v>23</v>
       </c>
       <c r="N12" s="2" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="O12" s="5">
         <v>0.34</v>
@@ -2563,10 +2563,10 @@
         <v>2</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="E13" s="3" t="s">
         <v>128</v>
@@ -2585,7 +2585,7 @@
         <v>26</v>
       </c>
       <c r="K13" s="3" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="L13" s="3" t="s">
         <v>24</v>
@@ -2594,7 +2594,7 @@
         <v>27</v>
       </c>
       <c r="N13" s="2" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="O13" s="5">
         <v>0.39</v>
@@ -2650,7 +2650,7 @@
         <v>4</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="D14" s="23" t="s">
         <v>136</v>
@@ -2668,16 +2668,16 @@
       <c r="I14" s="3"/>
       <c r="J14" s="3"/>
       <c r="K14" s="3" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="L14" s="3" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="M14" s="2" t="s">
         <v>101</v>
       </c>
       <c r="N14" s="2" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="O14" s="5">
         <v>0.47</v>
@@ -2733,7 +2733,7 @@
         <v>2</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="D15" s="23" t="s">
         <v>135</v>
@@ -2755,7 +2755,7 @@
         <v>26</v>
       </c>
       <c r="K15" s="3" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="L15" s="3" t="s">
         <v>31</v>
@@ -2764,7 +2764,7 @@
         <v>32</v>
       </c>
       <c r="N15" s="2" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="O15" s="5">
         <v>0.11</v>
@@ -2884,7 +2884,7 @@
         <v>36</v>
       </c>
       <c r="K17" s="3" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="L17" s="3" t="s">
         <v>37</v>
@@ -2893,7 +2893,7 @@
         <v>38</v>
       </c>
       <c r="N17" s="2" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="O17" s="5">
         <v>0.72</v>
@@ -2997,7 +2997,7 @@
         <v>1</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="D19" s="4" t="s">
         <v>112</v>
@@ -3015,7 +3015,7 @@
         <v>110</v>
       </c>
       <c r="K19" s="3" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="L19" s="3" t="s">
         <v>113</v>
@@ -3024,7 +3024,7 @@
         <v>109</v>
       </c>
       <c r="N19" s="2" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="O19" s="3">
         <v>0.40200000000000002</v>
@@ -3096,16 +3096,16 @@
       <c r="I20" s="3"/>
       <c r="J20" s="3"/>
       <c r="K20" s="3" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="L20" s="3" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="M20" s="2" t="s">
         <v>93</v>
       </c>
       <c r="N20" s="3" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="O20" s="5">
         <v>0.1</v>
@@ -3179,7 +3179,7 @@
         <v>106</v>
       </c>
       <c r="K21" s="3" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="L21" s="3" t="s">
         <v>105</v>
@@ -3188,7 +3188,7 @@
         <v>104</v>
       </c>
       <c r="N21" s="26" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="O21" s="6">
         <v>0.56000000000000005</v>
@@ -3213,7 +3213,7 @@
         <v>11.8</v>
       </c>
       <c r="U21" s="4" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="V21" s="4" t="str">
         <f t="shared" si="0"/>
@@ -3244,16 +3244,16 @@
         <v>1</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="F22" s="3" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="G22" s="3"/>
       <c r="H22" s="3"/>
@@ -3261,19 +3261,19 @@
         <v>1</v>
       </c>
       <c r="J22" s="3" t="s">
+        <v>182</v>
+      </c>
+      <c r="K22" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="L22" s="3" t="s">
         <v>183</v>
       </c>
-      <c r="K22" s="3" t="s">
-        <v>168</v>
-      </c>
-      <c r="L22" s="3" t="s">
-        <v>184</v>
-      </c>
       <c r="M22" s="15" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="N22" s="2" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="O22" s="6">
         <v>1.1299999999999999</v>
@@ -3372,7 +3372,7 @@
         <v>6</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="D24" s="23" t="s">
         <v>134</v>
@@ -3394,7 +3394,7 @@
         <v>40</v>
       </c>
       <c r="K24" s="3" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="L24" s="3" t="s">
         <v>92</v>
@@ -3403,7 +3403,7 @@
         <v>90</v>
       </c>
       <c r="N24" s="2" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="O24" s="6">
         <v>1.51</v>
@@ -3498,10 +3498,10 @@
         <v>1</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>259</v>
+        <v>255</v>
       </c>
       <c r="D26" s="4" t="s">
-        <v>259</v>
+        <v>255</v>
       </c>
       <c r="E26" s="3" t="s">
         <v>41</v>
@@ -3518,16 +3518,16 @@
         <v>43</v>
       </c>
       <c r="K26" s="3" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="L26" s="3" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="M26" s="2" t="s">
         <v>44</v>
       </c>
       <c r="N26" s="2" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="O26" s="5">
         <v>0.08</v>
@@ -3583,10 +3583,10 @@
         <v>13</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
       <c r="D27" s="23" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
       <c r="E27" s="3" t="s">
         <v>45</v>
@@ -3603,16 +3603,16 @@
         <v>43</v>
       </c>
       <c r="K27" s="3" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="L27" s="3" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="M27" s="2" t="s">
         <v>47</v>
       </c>
       <c r="N27" s="2" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="O27" s="5">
         <v>0.06</v>
@@ -3661,41 +3661,41 @@
     <row r="28" spans="1:26" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A28" s="19">
         <f>LEN(C28)-LEN(SUBSTITUTE(C28,",",""))+1</f>
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="B28" s="19">
         <f t="shared" si="21"/>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C28" s="12" t="s">
-        <v>242</v>
+        <v>260</v>
       </c>
       <c r="D28" s="24" t="s">
-        <v>140</v>
+        <v>262</v>
       </c>
       <c r="E28" s="13">
         <v>680</v>
       </c>
       <c r="F28" s="7" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="G28" s="3"/>
       <c r="H28" s="13"/>
       <c r="I28" s="13"/>
       <c r="J28" s="13" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="K28" s="13" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="L28" s="7" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="M28" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="N28" s="2" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="O28" s="14">
         <v>0.22</v>
@@ -3705,42 +3705,42 @@
       </c>
       <c r="Q28" s="6">
         <f t="shared" si="22"/>
-        <v>1.76</v>
+        <v>0.88</v>
       </c>
       <c r="R28" s="6">
         <f t="shared" si="4"/>
-        <v>1.2</v>
+        <v>0.6</v>
       </c>
       <c r="S28" s="6">
         <f t="shared" si="23"/>
-        <v>0.88</v>
+        <v>0.44</v>
       </c>
       <c r="T28" s="6">
         <f t="shared" si="5"/>
-        <v>0.6</v>
+        <v>0.3</v>
       </c>
       <c r="U28" s="12" t="s">
         <v>103</v>
       </c>
       <c r="V28" s="4" t="str">
         <f t="shared" si="19"/>
-        <v>8,A105963CT-ND</v>
+        <v>4,A105963CT-ND</v>
       </c>
       <c r="W28" s="4" t="str">
         <f t="shared" si="6"/>
-        <v>4,A105963CT-ND</v>
+        <v>2,A105963CT-ND</v>
       </c>
       <c r="X28" t="str">
         <f t="shared" si="24"/>
-        <v>Resistor - 8x 680</v>
+        <v>Resistor - 4x 680</v>
       </c>
       <c r="Y28" t="str">
         <f t="shared" si="8"/>
-        <v>279-LR1F680R|8</v>
+        <v>279-LR1F680R|4</v>
       </c>
       <c r="Z28" t="str">
         <f t="shared" si="9"/>
-        <v>1622545-1 8</v>
+        <v>1622545-1 4</v>
       </c>
     </row>
     <row r="29" spans="1:26" ht="27" thickBot="1" x14ac:dyDescent="0.25">
@@ -3753,10 +3753,10 @@
         <v>6</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="D29" s="4" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="E29" s="3">
         <v>470</v>
@@ -3773,7 +3773,7 @@
         <v>49</v>
       </c>
       <c r="K29" s="3" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="L29" s="7" t="s">
         <v>50</v>
@@ -3782,7 +3782,7 @@
         <v>51</v>
       </c>
       <c r="N29" s="2" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="O29" s="5">
         <v>0.11</v>
@@ -3831,23 +3831,23 @@
     <row r="30" spans="1:26" ht="27" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A30" s="19">
         <f t="shared" si="21"/>
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="B30" s="19">
         <f t="shared" si="21"/>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>256</v>
+        <v>261</v>
       </c>
       <c r="D30" s="4" t="s">
-        <v>257</v>
+        <v>263</v>
       </c>
       <c r="E30" s="3" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="F30" s="3" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="G30" s="3" t="s">
         <v>52</v>
@@ -3860,16 +3860,16 @@
         <v>43</v>
       </c>
       <c r="K30" s="3" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="L30" s="3" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="M30" s="2" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="N30" s="2" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="O30" s="5">
         <v>0.14000000000000001</v>
@@ -3879,40 +3879,40 @@
       </c>
       <c r="Q30" s="6">
         <f t="shared" si="22"/>
-        <v>0.42000000000000004</v>
+        <v>0.98000000000000009</v>
       </c>
       <c r="R30" s="6">
         <f t="shared" si="4"/>
-        <v>0.48</v>
+        <v>1.1200000000000001</v>
       </c>
       <c r="S30" s="6">
         <f t="shared" si="23"/>
-        <v>0.42000000000000004</v>
+        <v>0.70000000000000007</v>
       </c>
       <c r="T30" s="6">
         <f t="shared" si="5"/>
-        <v>0.48</v>
+        <v>0.8</v>
       </c>
       <c r="U30" s="4"/>
       <c r="V30" s="4" t="str">
         <f t="shared" si="19"/>
-        <v>3,2.49KXBK-ND</v>
+        <v>7,2.49KXBK-ND</v>
       </c>
       <c r="W30" s="4" t="str">
         <f t="shared" si="6"/>
-        <v>3,2.49KXBK-ND</v>
+        <v>5,2.49KXBK-ND</v>
       </c>
       <c r="X30" t="str">
         <f t="shared" si="24"/>
-        <v>Resistor - 3x 1% 2.49k</v>
+        <v>Resistor - 7x 1% 2.49k</v>
       </c>
       <c r="Y30" t="str">
         <f t="shared" si="8"/>
-        <v>603-MFR-25FBF52-2K49|3</v>
+        <v>603-MFR-25FBF52-2K49|7</v>
       </c>
       <c r="Z30" t="str">
         <f t="shared" si="9"/>
-        <v>MFR-25FBF52-2K49 3</v>
+        <v>MFR-25FBF52-2K49 7</v>
       </c>
     </row>
     <row r="31" spans="1:26" ht="17" thickBot="1" x14ac:dyDescent="0.25">
@@ -3944,7 +3944,7 @@
         <v>43</v>
       </c>
       <c r="K31" s="3" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="L31" s="3" t="s">
         <v>54</v>
@@ -3953,7 +3953,7 @@
         <v>55</v>
       </c>
       <c r="N31" s="2" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="O31" s="5">
         <v>0.46</v>
@@ -4011,7 +4011,7 @@
         <v>8</v>
       </c>
       <c r="C32" s="4" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="D32" s="23" t="s">
         <v>139</v>
@@ -4031,7 +4031,7 @@
         <v>43</v>
       </c>
       <c r="K32" s="3" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="L32" s="3" t="s">
         <v>58</v>
@@ -4040,7 +4040,7 @@
         <v>59</v>
       </c>
       <c r="N32" s="2" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="O32" s="5">
         <v>0.1</v>
@@ -4096,7 +4096,7 @@
         <v>2</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="D33" s="23" t="s">
         <v>137</v>
@@ -4116,7 +4116,7 @@
         <v>43</v>
       </c>
       <c r="K33" s="3" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="L33" s="3" t="s">
         <v>61</v>
@@ -4125,7 +4125,7 @@
         <v>62</v>
       </c>
       <c r="N33" s="2" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="O33" s="5">
         <v>0.27</v>
@@ -4241,7 +4241,7 @@
         <v>68</v>
       </c>
       <c r="K35" s="3" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="L35" s="3" t="s">
         <v>65</v>
@@ -4250,7 +4250,7 @@
         <v>65</v>
       </c>
       <c r="N35" s="2" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="O35" s="5">
         <v>1.68</v>
@@ -4328,13 +4328,13 @@
       </c>
       <c r="K36" s="3"/>
       <c r="L36" s="3" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="M36" s="2" t="s">
         <v>81</v>
       </c>
       <c r="N36" s="2" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="O36" s="6">
         <v>15.41</v>
@@ -4389,7 +4389,7 @@
         <v>1</v>
       </c>
       <c r="C37" s="12" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="D37" s="12" t="s">
         <v>138</v>
@@ -4411,7 +4411,7 @@
         <v>69</v>
       </c>
       <c r="K37" s="13" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="L37" s="13" t="s">
         <v>129</v>
@@ -4420,7 +4420,7 @@
         <v>132</v>
       </c>
       <c r="N37" s="13" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="O37" s="21">
         <v>2.92</v>
@@ -4474,16 +4474,16 @@
         <v>1</v>
       </c>
       <c r="C38" s="12" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="D38" s="12" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="E38" s="13" t="s">
+        <v>228</v>
+      </c>
+      <c r="F38" s="3" t="s">
         <v>229</v>
-      </c>
-      <c r="F38" s="3" t="s">
-        <v>230</v>
       </c>
       <c r="G38" s="3" t="s">
         <v>131</v>
@@ -4493,19 +4493,19 @@
         <v>1</v>
       </c>
       <c r="J38" s="13" t="s">
+        <v>230</v>
+      </c>
+      <c r="K38" s="28" t="s">
+        <v>167</v>
+      </c>
+      <c r="L38" s="13" t="s">
+        <v>228</v>
+      </c>
+      <c r="M38" s="13" t="s">
         <v>231</v>
       </c>
-      <c r="K38" s="28" t="s">
-        <v>168</v>
-      </c>
-      <c r="L38" s="13" t="s">
-        <v>229</v>
-      </c>
-      <c r="M38" s="13" t="s">
+      <c r="N38" s="2" t="s">
         <v>232</v>
-      </c>
-      <c r="N38" s="2" t="s">
-        <v>233</v>
       </c>
       <c r="O38" s="6">
         <v>2.4</v>
@@ -4573,7 +4573,7 @@
       <c r="I39" s="3"/>
       <c r="J39" s="3"/>
       <c r="K39" s="3" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="L39" s="3" t="s">
         <v>86</v>
@@ -4582,7 +4582,7 @@
         <v>85</v>
       </c>
       <c r="N39" s="2" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="O39" s="6">
         <v>0.5</v>
@@ -4671,10 +4671,10 @@
         <v>1</v>
       </c>
       <c r="C41" s="4" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D41" s="4" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="E41" s="3"/>
       <c r="F41" s="3"/>
@@ -4684,17 +4684,17 @@
         <v>1</v>
       </c>
       <c r="J41" s="3" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="K41" s="3"/>
       <c r="L41" s="3" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="M41" s="13" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="N41" s="13" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="O41" s="6">
         <v>15.33</v>
@@ -4804,10 +4804,10 @@
       </c>
       <c r="B44" s="17"/>
       <c r="C44" s="4" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="D44" s="4" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="E44" s="3" t="s">
         <v>73</v>
@@ -4908,19 +4908,19 @@
       <c r="P46" s="1"/>
       <c r="Q46" s="11">
         <f>SUM(Q2:Q45)</f>
-        <v>99.032000000000011</v>
+        <v>98.712000000000003</v>
       </c>
       <c r="R46" s="11">
         <f>SUM(R2:R45)</f>
-        <v>106.36000000000001</v>
+        <v>106.4</v>
       </c>
       <c r="S46" s="11">
         <f>SUM(S2:S45)</f>
-        <v>72.772000000000006</v>
+        <v>72.612000000000009</v>
       </c>
       <c r="T46" s="11">
         <f>SUM(T2:T45)</f>
-        <v>82.14</v>
+        <v>82.16</v>
       </c>
       <c r="U46" s="10" t="s">
         <v>71</v>

</xml_diff>

<commit_message>
Updated v0.4.3 BOM with in-stock part numbers
</commit_message>
<xml_diff>
--- a/reference/hardware/v0.4/BOMs/v0.4.3_bom.xlsx
+++ b/reference/hardware/v0.4/BOMs/v0.4.3_bom.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="28109"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="28209"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -261,9 +261,6 @@
     <t>RES 100K OHM 1/4W 1% METAL FILM</t>
   </si>
   <si>
-    <t>MFR-25FBF-100K</t>
-  </si>
-  <si>
     <t>100KXBK-ND</t>
   </si>
   <si>
@@ -357,15 +354,6 @@
     <t>C1,3,5,7,9,13,15</t>
   </si>
   <si>
-    <t>497-5896-5-ND</t>
-  </si>
-  <si>
-    <t>MOSFET N-CH 33V 62A TO-220</t>
-  </si>
-  <si>
-    <t>STP62NS04Z</t>
-  </si>
-  <si>
     <t>3M9580-ND</t>
   </si>
   <si>
@@ -402,9 +390,6 @@
     <t>S1012EC-40-ND</t>
   </si>
   <si>
-    <t>PREC040SAAN-RC</t>
-  </si>
-  <si>
     <t>Sullins Connector Solutions</t>
   </si>
   <si>
@@ -540,12 +525,6 @@
     <t>CAP CER 0.22UF 50V 10% RADIAL</t>
   </si>
   <si>
-    <t>399-4353-ND</t>
-  </si>
-  <si>
-    <t>C322C224K5R5TA</t>
-  </si>
-  <si>
     <t>CAP TANT 10UF 35V 10% RADIAL</t>
   </si>
   <si>
@@ -672,9 +651,6 @@
     <t>80-T356G106K035AT</t>
   </si>
   <si>
-    <t>80-C322C224K5R</t>
-  </si>
-  <si>
     <t>80-C322C104M5R-TR</t>
   </si>
   <si>
@@ -732,9 +708,6 @@
     <t>279-H83K9BDA</t>
   </si>
   <si>
-    <t>603-MFR-25FBF52-100K</t>
-  </si>
-  <si>
     <t>594-5083NW160R0J</t>
   </si>
   <si>
@@ -756,9 +729,6 @@
     <t>571-2828362</t>
   </si>
   <si>
-    <t>782-A000026</t>
-  </si>
-  <si>
     <t>Mouser price is crazy</t>
   </si>
   <si>
@@ -877,6 +847,36 @@
   </si>
   <si>
     <t>R1,3,R26,R28,R61</t>
+  </si>
+  <si>
+    <t>K224K20X7RF5UH5</t>
+  </si>
+  <si>
+    <t>BC2678CT-ND</t>
+  </si>
+  <si>
+    <t>594-K224K20X7RF5UH5</t>
+  </si>
+  <si>
+    <t>STP75NS04Z</t>
+  </si>
+  <si>
+    <t>497-5981-5-ND</t>
+  </si>
+  <si>
+    <t>MOSFET N-CH 33V TO-220</t>
+  </si>
+  <si>
+    <t>PREC040SAAN-RC..</t>
+  </si>
+  <si>
+    <t>571-41037410</t>
+  </si>
+  <si>
+    <t>MFR-25FBF52-100K</t>
+  </si>
+  <si>
+    <t>603-FMF-25FTF52100K</t>
   </si>
 </sst>
 </file>
@@ -886,7 +886,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00;[Red]\-&quot;$&quot;#,##0.00"/>
   </numFmts>
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -946,11 +946,6 @@
       <sz val="10"/>
       <color rgb="FFFF0000"/>
       <name val="Liberation Sans"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF333333"/>
-      <name val="Arial"/>
     </font>
   </fonts>
   <fills count="7">
@@ -1117,7 +1112,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1190,7 +1185,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="3" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1600,8 +1594,8 @@
   </sheetPr>
   <dimension ref="A1:Z46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="138" workbookViewId="0">
-      <selection activeCell="C30" sqref="C30"/>
+    <sheetView tabSelected="1" topLeftCell="E21" zoomScale="113" workbookViewId="0">
+      <selection activeCell="L35" sqref="L35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1623,16 +1617,16 @@
   <sheetData>
     <row r="1" spans="1:26" ht="27" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="16" t="s">
-        <v>169</v>
+        <v>162</v>
       </c>
       <c r="B1" s="16" t="s">
-        <v>170</v>
+        <v>163</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>172</v>
+        <v>165</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>0</v>
@@ -1644,7 +1638,7 @@
         <v>2</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>3</v>
@@ -1653,7 +1647,7 @@
         <v>4</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>166</v>
+        <v>159</v>
       </c>
       <c r="L1" s="1" t="s">
         <v>5</v>
@@ -1662,40 +1656,40 @@
         <v>6</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>188</v>
+        <v>181</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>189</v>
+        <v>182</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>190</v>
+        <v>183</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>217</v>
+        <v>208</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>218</v>
+        <v>209</v>
       </c>
       <c r="S1" s="1" t="s">
-        <v>225</v>
+        <v>215</v>
       </c>
       <c r="T1" s="1" t="s">
-        <v>226</v>
+        <v>216</v>
       </c>
       <c r="U1" s="1" t="s">
         <v>7</v>
       </c>
       <c r="V1" s="20" t="s">
-        <v>185</v>
+        <v>178</v>
       </c>
       <c r="W1" s="20" t="s">
-        <v>186</v>
+        <v>179</v>
       </c>
       <c r="X1" s="20" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="Y1" s="20" t="s">
-        <v>187</v>
+        <v>180</v>
       </c>
     </row>
     <row r="2" spans="1:26" ht="17" thickBot="1" x14ac:dyDescent="0.25">
@@ -1743,16 +1737,16 @@
         <v>1</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E3" s="3" t="s">
         <v>8</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>153</v>
+        <v>146</v>
       </c>
       <c r="G3" s="3" t="s">
         <v>9</v>
@@ -1765,16 +1759,16 @@
         <v>13</v>
       </c>
       <c r="K3" s="3" t="s">
-        <v>167</v>
+        <v>160</v>
       </c>
       <c r="L3" s="3" t="s">
-        <v>154</v>
+        <v>147</v>
       </c>
       <c r="M3" s="2" t="s">
-        <v>155</v>
+        <v>148</v>
       </c>
       <c r="N3" s="2" t="s">
-        <v>194</v>
+        <v>187</v>
       </c>
       <c r="O3" s="5">
         <v>1.7</v>
@@ -1830,16 +1824,16 @@
         <v>6</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>256</v>
+        <v>246</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>257</v>
+        <v>247</v>
       </c>
       <c r="E4" s="3" t="s">
         <v>11</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="G4" s="3" t="s">
         <v>12</v>
@@ -1852,16 +1846,16 @@
         <v>13</v>
       </c>
       <c r="K4" s="3" t="s">
-        <v>167</v>
+        <v>160</v>
       </c>
       <c r="L4" s="3" t="s">
-        <v>152</v>
+        <v>254</v>
       </c>
       <c r="M4" s="2" t="s">
-        <v>151</v>
+        <v>255</v>
       </c>
       <c r="N4" s="2" t="s">
-        <v>195</v>
+        <v>256</v>
       </c>
       <c r="O4" s="5">
         <v>0.66</v>
@@ -1888,11 +1882,11 @@
       <c r="U4" s="4"/>
       <c r="V4" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>6,399-4353-ND</v>
+        <v>6,BC2678CT-ND</v>
       </c>
       <c r="W4" s="4" t="str">
         <f t="shared" ref="W4:W41" si="6">IF(NOT(M4=""),B4&amp;","&amp;M4,"")</f>
-        <v>6,399-4353-ND</v>
+        <v>6,BC2678CT-ND</v>
       </c>
       <c r="X4" t="str">
         <f t="shared" ref="X4:X10" si="7">"Capacitor - " &amp;A4&amp;"x "&amp;E4</f>
@@ -1900,11 +1894,11 @@
       </c>
       <c r="Y4" t="str">
         <f t="shared" ref="Y4:Y41" si="8">IF(NOT(N4=""),N4&amp;"|"&amp;A4,"")</f>
-        <v>80-C322C224K5R|6</v>
+        <v>594-K224K20X7RF5UH5|6</v>
       </c>
       <c r="Z4" t="str">
         <f t="shared" ref="Z4:Z39" si="9">L4&amp;" "&amp;A4</f>
-        <v>C322C224K5R5TA 6</v>
+        <v>K224K20X7RF5UH5 6</v>
       </c>
     </row>
     <row r="5" spans="1:26" ht="27" thickBot="1" x14ac:dyDescent="0.25">
@@ -1917,16 +1911,16 @@
         <v>7</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>234</v>
+        <v>224</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E5" s="3" t="s">
         <v>14</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="G5" s="3" t="s">
         <v>12</v>
@@ -1939,16 +1933,16 @@
         <v>13</v>
       </c>
       <c r="K5" s="3" t="s">
-        <v>167</v>
+        <v>160</v>
       </c>
       <c r="L5" s="3" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
       <c r="M5" s="2" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
       <c r="N5" s="2" t="s">
-        <v>196</v>
+        <v>188</v>
       </c>
       <c r="O5" s="5">
         <v>0.32</v>
@@ -2004,16 +1998,16 @@
         <v>1</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E6" s="3" t="s">
         <v>15</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>156</v>
+        <v>149</v>
       </c>
       <c r="G6" s="3" t="s">
         <v>9</v>
@@ -2026,16 +2020,16 @@
         <v>13</v>
       </c>
       <c r="K6" s="3" t="s">
-        <v>167</v>
+        <v>160</v>
       </c>
       <c r="L6" s="3" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
       <c r="M6" s="2" t="s">
-        <v>158</v>
+        <v>151</v>
       </c>
       <c r="N6" s="2" t="s">
-        <v>197</v>
+        <v>189</v>
       </c>
       <c r="O6" s="5">
         <v>1.57</v>
@@ -2091,16 +2085,16 @@
         <v>1</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E7" s="3" t="s">
         <v>16</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>161</v>
+        <v>154</v>
       </c>
       <c r="G7" s="3" t="s">
         <v>12</v>
@@ -2113,16 +2107,16 @@
         <v>10</v>
       </c>
       <c r="K7" s="3" t="s">
-        <v>167</v>
+        <v>160</v>
       </c>
       <c r="L7" s="3" t="s">
-        <v>159</v>
+        <v>152</v>
       </c>
       <c r="M7" s="2" t="s">
-        <v>160</v>
+        <v>153</v>
       </c>
       <c r="N7" s="2" t="s">
-        <v>198</v>
+        <v>190</v>
       </c>
       <c r="O7" s="5">
         <v>0.62</v>
@@ -2178,16 +2172,16 @@
         <v>2</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>254</v>
+        <v>244</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>254</v>
+        <v>244</v>
       </c>
       <c r="E8" s="3" t="s">
         <v>17</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
       <c r="G8" s="3" t="s">
         <v>12</v>
@@ -2200,16 +2194,16 @@
         <v>13</v>
       </c>
       <c r="K8" s="3" t="s">
-        <v>167</v>
+        <v>160</v>
       </c>
       <c r="L8" s="3" t="s">
-        <v>163</v>
+        <v>156</v>
       </c>
       <c r="M8" s="2" t="s">
-        <v>164</v>
+        <v>157</v>
       </c>
       <c r="N8" s="2" t="s">
-        <v>199</v>
+        <v>191</v>
       </c>
       <c r="O8" s="5">
         <v>0.24</v>
@@ -2265,16 +2259,16 @@
         <v>2</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>235</v>
+        <v>225</v>
       </c>
       <c r="D9" s="23" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="E9" s="3" t="s">
         <v>18</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="G9" s="3" t="s">
         <v>12</v>
@@ -2287,16 +2281,16 @@
         <v>13</v>
       </c>
       <c r="K9" s="3" t="s">
-        <v>167</v>
+        <v>160</v>
       </c>
       <c r="L9" s="3" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="M9" s="2" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="N9" s="2" t="s">
-        <v>200</v>
+        <v>192</v>
       </c>
       <c r="O9" s="5">
         <v>0.66</v>
@@ -2352,16 +2346,16 @@
         <v>1</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="G10" s="3" t="s">
         <v>12</v>
@@ -2372,16 +2366,16 @@
         <v>13</v>
       </c>
       <c r="K10" s="3" t="s">
-        <v>167</v>
+        <v>160</v>
       </c>
       <c r="L10" s="3" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="M10" s="2" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="N10" s="2" t="s">
-        <v>201</v>
+        <v>193</v>
       </c>
       <c r="O10" s="5">
         <v>0.25</v>
@@ -2476,13 +2470,13 @@
         <v>1</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="F12" s="7" t="s">
         <v>19</v>
@@ -2498,7 +2492,7 @@
         <v>21</v>
       </c>
       <c r="K12" s="3" t="s">
-        <v>167</v>
+        <v>160</v>
       </c>
       <c r="L12" s="7" t="s">
         <v>22</v>
@@ -2507,7 +2501,7 @@
         <v>23</v>
       </c>
       <c r="N12" s="2" t="s">
-        <v>227</v>
+        <v>217</v>
       </c>
       <c r="O12" s="5">
         <v>0.34</v>
@@ -2563,13 +2557,13 @@
         <v>2</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>236</v>
+        <v>226</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>233</v>
+        <v>223</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="F13" s="3" t="s">
         <v>25</v>
@@ -2585,7 +2579,7 @@
         <v>26</v>
       </c>
       <c r="K13" s="3" t="s">
-        <v>168</v>
+        <v>161</v>
       </c>
       <c r="L13" s="3" t="s">
         <v>24</v>
@@ -2594,7 +2588,7 @@
         <v>27</v>
       </c>
       <c r="N13" s="2" t="s">
-        <v>202</v>
+        <v>194</v>
       </c>
       <c r="O13" s="5">
         <v>0.39</v>
@@ -2650,34 +2644,34 @@
         <v>4</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>237</v>
+        <v>227</v>
       </c>
       <c r="D14" s="23" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="E14" s="3" t="s">
         <v>28</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="G14" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="H14" s="3"/>
       <c r="I14" s="3"/>
       <c r="J14" s="3"/>
       <c r="K14" s="3" t="s">
-        <v>168</v>
+        <v>161</v>
       </c>
       <c r="L14" s="3" t="s">
-        <v>246</v>
+        <v>236</v>
       </c>
       <c r="M14" s="2" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="N14" s="2" t="s">
-        <v>219</v>
+        <v>210</v>
       </c>
       <c r="O14" s="5">
         <v>0.47</v>
@@ -2733,10 +2727,10 @@
         <v>2</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>238</v>
+        <v>228</v>
       </c>
       <c r="D15" s="23" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="E15" s="3" t="s">
         <v>29</v>
@@ -2755,7 +2749,7 @@
         <v>26</v>
       </c>
       <c r="K15" s="3" t="s">
-        <v>167</v>
+        <v>160</v>
       </c>
       <c r="L15" s="3" t="s">
         <v>31</v>
@@ -2764,7 +2758,7 @@
         <v>32</v>
       </c>
       <c r="N15" s="2" t="s">
-        <v>203</v>
+        <v>195</v>
       </c>
       <c r="O15" s="5">
         <v>0.11</v>
@@ -2862,10 +2856,10 @@
         <v>1</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="E17" s="3" t="s">
         <v>33</v>
@@ -2884,7 +2878,7 @@
         <v>36</v>
       </c>
       <c r="K17" s="3" t="s">
-        <v>168</v>
+        <v>161</v>
       </c>
       <c r="L17" s="3" t="s">
         <v>37</v>
@@ -2893,7 +2887,7 @@
         <v>38</v>
       </c>
       <c r="N17" s="2" t="s">
-        <v>204</v>
+        <v>196</v>
       </c>
       <c r="O17" s="5">
         <v>0.72</v>
@@ -2997,34 +2991,34 @@
         <v>1</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>239</v>
+        <v>229</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="F19" s="3" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="G19" s="3"/>
       <c r="H19" s="3"/>
       <c r="I19" s="3"/>
       <c r="J19" s="3" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="K19" s="3" t="s">
-        <v>168</v>
+        <v>161</v>
       </c>
       <c r="L19" s="3" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="M19" s="2" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="N19" s="2" t="s">
-        <v>222</v>
+        <v>213</v>
       </c>
       <c r="O19" s="3">
         <v>0.40200000000000002</v>
@@ -3049,7 +3043,7 @@
         <v>0.51</v>
       </c>
       <c r="U19" s="4" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="V19" s="4" t="str">
         <f t="shared" si="0"/>
@@ -3080,32 +3074,32 @@
         <v>5</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="E20" s="3" t="s">
         <v>39</v>
       </c>
       <c r="F20" s="3" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="G20" s="3"/>
       <c r="H20" s="3"/>
       <c r="I20" s="3"/>
       <c r="J20" s="3"/>
       <c r="K20" s="3" t="s">
-        <v>168</v>
+        <v>161</v>
       </c>
       <c r="L20" s="3" t="s">
-        <v>208</v>
+        <v>200</v>
       </c>
       <c r="M20" s="2" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="N20" s="3" t="s">
-        <v>207</v>
+        <v>199</v>
       </c>
       <c r="O20" s="5">
         <v>0.1</v>
@@ -3159,16 +3153,16 @@
         <v>4</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="D21" s="4" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="F21" s="3" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="G21" s="3"/>
       <c r="H21" s="3"/>
@@ -3176,24 +3170,24 @@
         <v>1</v>
       </c>
       <c r="J21" s="3" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="K21" s="3" t="s">
-        <v>168</v>
+        <v>161</v>
       </c>
       <c r="L21" s="3" t="s">
-        <v>105</v>
+        <v>260</v>
       </c>
       <c r="M21" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="N21" s="26" t="s">
-        <v>223</v>
+        <v>100</v>
+      </c>
+      <c r="N21" s="2" t="s">
+        <v>261</v>
       </c>
       <c r="O21" s="6">
         <v>0.56000000000000005</v>
       </c>
-      <c r="P21" s="27">
+      <c r="P21" s="26">
         <v>2.95</v>
       </c>
       <c r="Q21" s="6">
@@ -3213,7 +3207,7 @@
         <v>11.8</v>
       </c>
       <c r="U21" s="4" t="s">
-        <v>224</v>
+        <v>214</v>
       </c>
       <c r="V21" s="4" t="str">
         <f t="shared" si="0"/>
@@ -3229,11 +3223,11 @@
       </c>
       <c r="Y21" t="str">
         <f t="shared" si="8"/>
-        <v>782-A000026|4</v>
+        <v>571-41037410|4</v>
       </c>
       <c r="Z21" t="str">
         <f t="shared" si="9"/>
-        <v>PREC040SAAN-RC 4</v>
+        <v>PREC040SAAN-RC.. 4</v>
       </c>
     </row>
     <row r="22" spans="1:26" ht="40" thickBot="1" x14ac:dyDescent="0.25">
@@ -3244,16 +3238,16 @@
         <v>1</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>184</v>
+        <v>177</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>184</v>
+        <v>177</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>181</v>
+        <v>174</v>
       </c>
       <c r="F22" s="3" t="s">
-        <v>180</v>
+        <v>173</v>
       </c>
       <c r="G22" s="3"/>
       <c r="H22" s="3"/>
@@ -3261,19 +3255,19 @@
         <v>1</v>
       </c>
       <c r="J22" s="3" t="s">
-        <v>182</v>
+        <v>175</v>
       </c>
       <c r="K22" s="3" t="s">
-        <v>167</v>
+        <v>160</v>
       </c>
       <c r="L22" s="3" t="s">
-        <v>183</v>
+        <v>176</v>
       </c>
       <c r="M22" s="15" t="s">
-        <v>179</v>
+        <v>172</v>
       </c>
       <c r="N22" s="2" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="O22" s="6">
         <v>1.1299999999999999</v>
@@ -3372,19 +3366,19 @@
         <v>6</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>240</v>
+        <v>230</v>
       </c>
       <c r="D24" s="23" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="F24" s="3" t="s">
-        <v>91</v>
+        <v>259</v>
       </c>
       <c r="G24" s="3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="H24" s="3"/>
       <c r="I24" s="3">
@@ -3394,16 +3388,16 @@
         <v>40</v>
       </c>
       <c r="K24" s="3" t="s">
-        <v>167</v>
+        <v>160</v>
       </c>
       <c r="L24" s="3" t="s">
-        <v>92</v>
+        <v>257</v>
       </c>
       <c r="M24" s="2" t="s">
-        <v>90</v>
+        <v>258</v>
       </c>
       <c r="N24" s="2" t="s">
-        <v>205</v>
+        <v>197</v>
       </c>
       <c r="O24" s="6">
         <v>1.51</v>
@@ -3430,11 +3424,11 @@
       <c r="U24" s="4"/>
       <c r="V24" s="4" t="str">
         <f t="shared" si="19"/>
-        <v>8,497-5896-5-ND</v>
+        <v>8,497-5981-5-ND</v>
       </c>
       <c r="W24" s="4" t="str">
         <f>IF(NOT(M24=""),B24&amp;","&amp;M24,"")</f>
-        <v>6,497-5896-5-ND</v>
+        <v>6,497-5981-5-ND</v>
       </c>
       <c r="X24" t="str">
         <f t="shared" si="13"/>
@@ -3446,7 +3440,7 @@
       </c>
       <c r="Z24" t="str">
         <f t="shared" si="9"/>
-        <v>STP62NS04Z 8</v>
+        <v>STP75NS04Z 8</v>
       </c>
     </row>
     <row r="25" spans="1:26" ht="17" thickBot="1" x14ac:dyDescent="0.25">
@@ -3498,10 +3492,10 @@
         <v>1</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>255</v>
+        <v>245</v>
       </c>
       <c r="D26" s="4" t="s">
-        <v>255</v>
+        <v>245</v>
       </c>
       <c r="E26" s="3" t="s">
         <v>41</v>
@@ -3518,16 +3512,16 @@
         <v>43</v>
       </c>
       <c r="K26" s="3" t="s">
-        <v>167</v>
+        <v>160</v>
       </c>
       <c r="L26" s="3" t="s">
-        <v>248</v>
+        <v>238</v>
       </c>
       <c r="M26" s="2" t="s">
         <v>44</v>
       </c>
       <c r="N26" s="2" t="s">
-        <v>210</v>
+        <v>202</v>
       </c>
       <c r="O26" s="5">
         <v>0.08</v>
@@ -3583,10 +3577,10 @@
         <v>13</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>258</v>
+        <v>248</v>
       </c>
       <c r="D27" s="23" t="s">
-        <v>259</v>
+        <v>249</v>
       </c>
       <c r="E27" s="3" t="s">
         <v>45</v>
@@ -3603,16 +3597,16 @@
         <v>43</v>
       </c>
       <c r="K27" s="3" t="s">
-        <v>167</v>
+        <v>160</v>
       </c>
       <c r="L27" s="3" t="s">
-        <v>247</v>
+        <v>237</v>
       </c>
       <c r="M27" s="2" t="s">
         <v>47</v>
       </c>
       <c r="N27" s="2" t="s">
-        <v>211</v>
+        <v>203</v>
       </c>
       <c r="O27" s="5">
         <v>0.06</v>
@@ -3668,34 +3662,34 @@
         <v>2</v>
       </c>
       <c r="C28" s="12" t="s">
-        <v>260</v>
+        <v>250</v>
       </c>
       <c r="D28" s="24" t="s">
-        <v>262</v>
+        <v>252</v>
       </c>
       <c r="E28" s="13">
         <v>680</v>
       </c>
       <c r="F28" s="7" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
       <c r="G28" s="3"/>
       <c r="H28" s="13"/>
       <c r="I28" s="13"/>
       <c r="J28" s="13" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="K28" s="13" t="s">
-        <v>167</v>
+        <v>160</v>
       </c>
       <c r="L28" s="7" t="s">
-        <v>245</v>
+        <v>235</v>
       </c>
       <c r="M28" s="2" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="N28" s="2" t="s">
-        <v>212</v>
+        <v>204</v>
       </c>
       <c r="O28" s="14">
         <v>0.22</v>
@@ -3720,7 +3714,7 @@
         <v>0.3</v>
       </c>
       <c r="U28" s="12" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="V28" s="4" t="str">
         <f t="shared" si="19"/>
@@ -3753,10 +3747,10 @@
         <v>6</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>241</v>
+        <v>231</v>
       </c>
       <c r="D29" s="4" t="s">
-        <v>165</v>
+        <v>158</v>
       </c>
       <c r="E29" s="3">
         <v>470</v>
@@ -3773,7 +3767,7 @@
         <v>49</v>
       </c>
       <c r="K29" s="3" t="s">
-        <v>167</v>
+        <v>160</v>
       </c>
       <c r="L29" s="7" t="s">
         <v>50</v>
@@ -3782,7 +3776,7 @@
         <v>51</v>
       </c>
       <c r="N29" s="2" t="s">
-        <v>213</v>
+        <v>205</v>
       </c>
       <c r="O29" s="5">
         <v>0.11</v>
@@ -3838,16 +3832,16 @@
         <v>5</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>261</v>
+        <v>251</v>
       </c>
       <c r="D30" s="4" t="s">
-        <v>263</v>
+        <v>253</v>
       </c>
       <c r="E30" s="3" t="s">
-        <v>250</v>
+        <v>240</v>
       </c>
       <c r="F30" s="3" t="s">
-        <v>251</v>
+        <v>241</v>
       </c>
       <c r="G30" s="3" t="s">
         <v>52</v>
@@ -3860,16 +3854,16 @@
         <v>43</v>
       </c>
       <c r="K30" s="3" t="s">
-        <v>167</v>
+        <v>160</v>
       </c>
       <c r="L30" s="3" t="s">
-        <v>252</v>
+        <v>242</v>
       </c>
       <c r="M30" s="2" t="s">
-        <v>249</v>
+        <v>239</v>
       </c>
       <c r="N30" s="2" t="s">
-        <v>253</v>
+        <v>243</v>
       </c>
       <c r="O30" s="5">
         <v>0.14000000000000001</v>
@@ -3924,13 +3918,13 @@
         <v>1</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D31" s="4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E31" s="3" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="F31" s="3" t="s">
         <v>53</v>
@@ -3944,7 +3938,7 @@
         <v>43</v>
       </c>
       <c r="K31" s="3" t="s">
-        <v>167</v>
+        <v>160</v>
       </c>
       <c r="L31" s="3" t="s">
         <v>54</v>
@@ -3953,7 +3947,7 @@
         <v>55</v>
       </c>
       <c r="N31" s="2" t="s">
-        <v>214</v>
+        <v>206</v>
       </c>
       <c r="O31" s="5">
         <v>0.46</v>
@@ -3978,7 +3972,7 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="U31" s="4" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="V31" s="4" t="str">
         <f t="shared" si="19"/>
@@ -4011,10 +4005,10 @@
         <v>8</v>
       </c>
       <c r="C32" s="4" t="s">
-        <v>242</v>
+        <v>232</v>
       </c>
       <c r="D32" s="23" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="E32" s="3" t="s">
         <v>56</v>
@@ -4031,16 +4025,16 @@
         <v>43</v>
       </c>
       <c r="K32" s="3" t="s">
-        <v>167</v>
+        <v>160</v>
       </c>
       <c r="L32" s="3" t="s">
+        <v>262</v>
+      </c>
+      <c r="M32" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="M32" s="2" t="s">
-        <v>59</v>
-      </c>
       <c r="N32" s="2" t="s">
-        <v>215</v>
+        <v>263</v>
       </c>
       <c r="O32" s="5">
         <v>0.1</v>
@@ -4079,11 +4073,11 @@
       </c>
       <c r="Y32" t="str">
         <f t="shared" si="8"/>
-        <v>603-MFR-25FBF52-100K|12</v>
+        <v>603-FMF-25FTF52100K|12</v>
       </c>
       <c r="Z32" t="str">
         <f t="shared" si="9"/>
-        <v>MFR-25FBF-100K 12</v>
+        <v>MFR-25FBF52-100K 12</v>
       </c>
     </row>
     <row r="33" spans="1:26" ht="17" thickBot="1" x14ac:dyDescent="0.25">
@@ -4096,16 +4090,16 @@
         <v>2</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>243</v>
+        <v>233</v>
       </c>
       <c r="D33" s="23" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="E33" s="3">
         <v>160</v>
       </c>
       <c r="F33" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="G33" s="3"/>
       <c r="H33" s="3"/>
@@ -4116,16 +4110,16 @@
         <v>43</v>
       </c>
       <c r="K33" s="3" t="s">
-        <v>167</v>
+        <v>160</v>
       </c>
       <c r="L33" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="M33" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="M33" s="2" t="s">
-        <v>62</v>
-      </c>
       <c r="N33" s="2" t="s">
-        <v>216</v>
+        <v>207</v>
       </c>
       <c r="O33" s="5">
         <v>0.27</v>
@@ -4219,38 +4213,38 @@
         <v>1</v>
       </c>
       <c r="C35" s="4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D35" s="4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E35" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="F35" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="F35" s="3" t="s">
+      <c r="G35" s="3" t="s">
         <v>66</v>
-      </c>
-      <c r="G35" s="3" t="s">
-        <v>67</v>
       </c>
       <c r="H35" s="3"/>
       <c r="I35" s="3">
         <v>2</v>
       </c>
       <c r="J35" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="K35" s="3" t="s">
-        <v>167</v>
+        <v>160</v>
       </c>
       <c r="L35" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="M35" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="N35" s="2" t="s">
-        <v>206</v>
+        <v>198</v>
       </c>
       <c r="O35" s="5">
         <v>1.68</v>
@@ -4305,36 +4299,36 @@
         <v>1</v>
       </c>
       <c r="C36" s="4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D36" s="4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E36" s="3" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="F36" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="G36" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="H36" s="3"/>
       <c r="I36" s="3">
         <v>1</v>
       </c>
       <c r="J36" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="K36" s="3"/>
       <c r="L36" s="3" t="s">
-        <v>191</v>
+        <v>184</v>
       </c>
       <c r="M36" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="N36" s="2" t="s">
-        <v>192</v>
+        <v>185</v>
       </c>
       <c r="O36" s="6">
         <v>15.41</v>
@@ -4389,38 +4383,38 @@
         <v>1</v>
       </c>
       <c r="C37" s="12" t="s">
-        <v>244</v>
+        <v>234</v>
       </c>
       <c r="D37" s="12" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="E37" s="13" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="F37" s="13" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="G37" s="3" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="H37" s="13"/>
       <c r="I37" s="13">
         <v>2</v>
       </c>
       <c r="J37" s="13" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="K37" s="13" t="s">
-        <v>167</v>
+        <v>160</v>
       </c>
       <c r="L37" s="13" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="M37" s="13" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="N37" s="13" t="s">
-        <v>193</v>
+        <v>186</v>
       </c>
       <c r="O37" s="21">
         <v>2.92</v>
@@ -4470,42 +4464,42 @@
       <c r="A38" s="19">
         <v>1</v>
       </c>
-      <c r="B38" s="29">
+      <c r="B38" s="28">
         <v>1</v>
       </c>
       <c r="C38" s="12" t="s">
-        <v>176</v>
+        <v>169</v>
       </c>
       <c r="D38" s="12" t="s">
-        <v>176</v>
+        <v>169</v>
       </c>
       <c r="E38" s="13" t="s">
-        <v>228</v>
+        <v>218</v>
       </c>
       <c r="F38" s="3" t="s">
-        <v>229</v>
+        <v>219</v>
       </c>
       <c r="G38" s="3" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="H38" s="13"/>
       <c r="I38" s="13">
         <v>1</v>
       </c>
       <c r="J38" s="13" t="s">
-        <v>230</v>
-      </c>
-      <c r="K38" s="28" t="s">
-        <v>167</v>
+        <v>220</v>
+      </c>
+      <c r="K38" s="27" t="s">
+        <v>160</v>
       </c>
       <c r="L38" s="13" t="s">
-        <v>228</v>
+        <v>218</v>
       </c>
       <c r="M38" s="13" t="s">
-        <v>231</v>
+        <v>221</v>
       </c>
       <c r="N38" s="2" t="s">
-        <v>232</v>
+        <v>222</v>
       </c>
       <c r="O38" s="6">
         <v>2.4</v>
@@ -4559,13 +4553,13 @@
         <v>2</v>
       </c>
       <c r="C39" s="15" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D39" s="15" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E39" s="3" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="F39" s="3"/>
       <c r="G39" s="3"/>
@@ -4573,16 +4567,16 @@
       <c r="I39" s="3"/>
       <c r="J39" s="3"/>
       <c r="K39" s="3" t="s">
-        <v>167</v>
+        <v>160</v>
       </c>
       <c r="L39" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="M39" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="N39" s="2" t="s">
-        <v>221</v>
+        <v>212</v>
       </c>
       <c r="O39" s="6">
         <v>0.5</v>
@@ -4671,10 +4665,10 @@
         <v>1</v>
       </c>
       <c r="C41" s="4" t="s">
-        <v>177</v>
+        <v>170</v>
       </c>
       <c r="D41" s="4" t="s">
-        <v>177</v>
+        <v>170</v>
       </c>
       <c r="E41" s="3"/>
       <c r="F41" s="3"/>
@@ -4684,17 +4678,17 @@
         <v>1</v>
       </c>
       <c r="J41" s="3" t="s">
-        <v>175</v>
+        <v>168</v>
       </c>
       <c r="K41" s="3"/>
       <c r="L41" s="3" t="s">
-        <v>174</v>
+        <v>167</v>
       </c>
       <c r="M41" s="13" t="s">
-        <v>173</v>
+        <v>166</v>
       </c>
       <c r="N41" s="13" t="s">
-        <v>220</v>
+        <v>211</v>
       </c>
       <c r="O41" s="6">
         <v>15.33</v>
@@ -4767,10 +4761,10 @@
       <c r="A43" s="17"/>
       <c r="B43" s="17"/>
       <c r="C43" s="4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D43" s="4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E43" s="3"/>
       <c r="F43" s="3"/>
@@ -4804,13 +4798,13 @@
       </c>
       <c r="B44" s="17"/>
       <c r="C44" s="4" t="s">
-        <v>178</v>
+        <v>171</v>
       </c>
       <c r="D44" s="4" t="s">
-        <v>178</v>
+        <v>171</v>
       </c>
       <c r="E44" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F44" s="3"/>
       <c r="G44" s="3"/>
@@ -4819,11 +4813,11 @@
         <v>1</v>
       </c>
       <c r="J44" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="K44" s="3"/>
       <c r="L44" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="M44" s="3"/>
       <c r="N44" s="3"/>
@@ -4856,10 +4850,10 @@
       </c>
       <c r="B45" s="17"/>
       <c r="C45" s="4" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="D45" s="4" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="E45" s="3"/>
       <c r="F45" s="3"/>
@@ -4870,7 +4864,7 @@
       <c r="K45" s="3"/>
       <c r="L45" s="3"/>
       <c r="M45" s="3" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="N45" s="3"/>
       <c r="O45" s="3">
@@ -4882,7 +4876,7 @@
       <c r="S45" s="6"/>
       <c r="T45" s="6"/>
       <c r="U45" s="4" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
     </row>
     <row r="46" spans="1:26" ht="17" thickBot="1" x14ac:dyDescent="0.25">
@@ -4897,13 +4891,13 @@
       <c r="I46" s="8"/>
       <c r="J46" s="4"/>
       <c r="K46" s="8"/>
-      <c r="L46" s="30" t="s">
-        <v>75</v>
-      </c>
-      <c r="M46" s="31"/>
+      <c r="L46" s="29" t="s">
+        <v>74</v>
+      </c>
+      <c r="M46" s="30"/>
       <c r="N46" s="25"/>
       <c r="O46" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="P46" s="1"/>
       <c r="Q46" s="11">
@@ -4923,7 +4917,7 @@
         <v>82.16</v>
       </c>
       <c r="U46" s="10" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
   </sheetData>
@@ -4938,11 +4932,11 @@
     <hyperlink ref="M26" r:id="rId4"/>
     <hyperlink ref="M30" r:id="rId5" display="985-1047-1-ND"/>
     <hyperlink ref="M31" r:id="rId6"/>
-    <hyperlink ref="M32" r:id="rId7"/>
-    <hyperlink ref="M36" r:id="rId8"/>
-    <hyperlink ref="M3" r:id="rId9" display="478-1842-ND"/>
-    <hyperlink ref="M7" r:id="rId10" display="445-5312-ND"/>
-    <hyperlink ref="M8" r:id="rId11" display="399-4148-ND"/>
+    <hyperlink ref="M36" r:id="rId7"/>
+    <hyperlink ref="M3" r:id="rId8" display="478-1842-ND"/>
+    <hyperlink ref="M7" r:id="rId9" display="445-5312-ND"/>
+    <hyperlink ref="M8" r:id="rId10" display="399-4148-ND"/>
+    <hyperlink ref="M32" r:id="rId11"/>
   </hyperlinks>
   <pageMargins left="0.75000000000000011" right="0.75000000000000011" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" scale="21" orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292" copies="2"/>

</xml_diff>

<commit_message>
Cleanup of hardware directory
</commit_message>
<xml_diff>
--- a/reference/hardware/v0.4/BOMs/v0.4.3_bom.xlsx
+++ b/reference/hardware/v0.4/BOMs/v0.4.3_bom.xlsx
@@ -1,24 +1,30 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10210"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11110"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/josh/Documents/Arduino/speeduino/reference/hardware/v0.4/BOMs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD2EE3F3-356B-CE47-8295-B0FB53071B1D}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F0AFFD5-2611-D043-902D-0E690169F52E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16520" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16100" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Component List" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="171027" concurrentCalc="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
     </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -86,7 +92,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="339" uniqueCount="264">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="339" uniqueCount="265">
   <si>
     <t>Value</t>
   </si>
@@ -517,12 +523,6 @@
     <t>CAP CER 0.1UF 50V 20% RADIAL</t>
   </si>
   <si>
-    <t>C322C104M5R5TA7301</t>
-  </si>
-  <si>
-    <t>399-9879-1-ND</t>
-  </si>
-  <si>
     <t>CAP CER 0.22UF 50V 10% RADIAL</t>
   </si>
   <si>
@@ -878,6 +878,15 @@
   </si>
   <si>
     <t>603-FMF-25FTF52100K</t>
+  </si>
+  <si>
+    <t>Vishay</t>
+  </si>
+  <si>
+    <t>K104K15X7RF53H5</t>
+  </si>
+  <si>
+    <t>BC3323-ND</t>
   </si>
 </sst>
 </file>
@@ -887,7 +896,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00;[Red]\-&quot;$&quot;#,##0.00"/>
   </numFmts>
-  <fonts count="10">
+  <fonts count="9">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -924,12 +933,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="9"/>
@@ -1114,7 +1117,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1158,7 +1161,6 @@
     <xf numFmtId="164" fontId="3" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1178,10 +1180,10 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1599,14 +1601,14 @@
   </sheetPr>
   <dimension ref="A1:Z46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="113" workbookViewId="0">
-      <selection activeCell="F38" sqref="F38"/>
+    <sheetView tabSelected="1" zoomScale="113" workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="1" width="18.83203125" style="18" customWidth="1"/>
-    <col min="2" max="2" width="18.83203125" style="18" hidden="1" customWidth="1"/>
+    <col min="1" max="1" width="18.83203125" style="17" customWidth="1"/>
+    <col min="2" max="2" width="18.83203125" style="17" hidden="1" customWidth="1"/>
     <col min="3" max="3" width="46.6640625" customWidth="1"/>
     <col min="4" max="4" width="46.6640625" hidden="1" customWidth="1"/>
     <col min="5" max="5" width="15" customWidth="1"/>
@@ -1622,18 +1624,18 @@
     <col min="25" max="25" width="22.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" ht="27" thickBot="1">
-      <c r="A1" s="16" t="s">
+    <row r="1" spans="1:26" ht="29" thickBot="1">
+      <c r="A1" s="15" t="s">
+        <v>160</v>
+      </c>
+      <c r="B1" s="15" t="s">
+        <v>161</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>162</v>
       </c>
-      <c r="B1" s="16" t="s">
+      <c r="D1" s="1" t="s">
         <v>163</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>164</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>165</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>0</v>
@@ -1654,7 +1656,7 @@
         <v>4</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="L1" s="1" t="s">
         <v>5</v>
@@ -1663,45 +1665,45 @@
         <v>6</v>
       </c>
       <c r="N1" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="P1" s="1" t="s">
         <v>181</v>
       </c>
-      <c r="O1" s="1" t="s">
-        <v>182</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>183</v>
-      </c>
       <c r="Q1" s="1" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="S1" s="1" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="T1" s="1" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="U1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="V1" s="20" t="s">
+      <c r="V1" s="19" t="s">
+        <v>176</v>
+      </c>
+      <c r="W1" s="19" t="s">
+        <v>177</v>
+      </c>
+      <c r="X1" s="19" t="s">
+        <v>120</v>
+      </c>
+      <c r="Y1" s="19" t="s">
         <v>178</v>
-      </c>
-      <c r="W1" s="20" t="s">
-        <v>179</v>
-      </c>
-      <c r="X1" s="20" t="s">
-        <v>120</v>
-      </c>
-      <c r="Y1" s="20" t="s">
-        <v>180</v>
       </c>
     </row>
     <row r="2" spans="1:26" ht="17" thickBot="1">
-      <c r="A2" s="17"/>
-      <c r="B2" s="17"/>
+      <c r="A2" s="16"/>
+      <c r="B2" s="16"/>
       <c r="C2" s="4"/>
       <c r="D2" s="4"/>
       <c r="E2" s="3"/>
@@ -1735,11 +1737,11 @@
       </c>
     </row>
     <row r="3" spans="1:26" ht="17" thickBot="1">
-      <c r="A3" s="19">
+      <c r="A3" s="18">
         <f>LEN(C3)-LEN(SUBSTITUTE(C3,",",""))+1</f>
         <v>1</v>
       </c>
-      <c r="B3" s="19">
+      <c r="B3" s="18">
         <f t="shared" ref="B3:B10" si="1">LEN(D3)-LEN(SUBSTITUTE(D3,",",""))+1</f>
         <v>1</v>
       </c>
@@ -1753,7 +1755,7 @@
         <v>8</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="G3" s="3" t="s">
         <v>9</v>
@@ -1766,16 +1768,16 @@
         <v>13</v>
       </c>
       <c r="K3" s="3" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="L3" s="3" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="M3" s="2" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="N3" s="2" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="O3" s="5">
         <v>1.7</v>
@@ -1822,25 +1824,25 @@
       </c>
     </row>
     <row r="4" spans="1:26" ht="17" thickBot="1">
-      <c r="A4" s="19">
+      <c r="A4" s="18">
         <f>LEN(C4)-LEN(SUBSTITUTE(C4,",",""))+1</f>
         <v>6</v>
       </c>
-      <c r="B4" s="19">
+      <c r="B4" s="18">
         <f t="shared" si="1"/>
         <v>6</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="E4" s="3" t="s">
         <v>11</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="G4" s="3" t="s">
         <v>12</v>
@@ -1853,16 +1855,16 @@
         <v>13</v>
       </c>
       <c r="K4" s="3" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="L4" s="3" t="s">
+        <v>252</v>
+      </c>
+      <c r="M4" s="2" t="s">
+        <v>253</v>
+      </c>
+      <c r="N4" s="2" t="s">
         <v>254</v>
-      </c>
-      <c r="M4" s="2" t="s">
-        <v>255</v>
-      </c>
-      <c r="N4" s="2" t="s">
-        <v>256</v>
       </c>
       <c r="O4" s="5">
         <v>0.66</v>
@@ -1908,17 +1910,17 @@
         <v>K224K20X7RF5UH5 6</v>
       </c>
     </row>
-    <row r="5" spans="1:26" ht="27" thickBot="1">
-      <c r="A5" s="19">
+    <row r="5" spans="1:26" ht="17" thickBot="1">
+      <c r="A5" s="18">
         <f>LEN(C5)-LEN(SUBSTITUTE(C5,",",""))+1</f>
         <v>7</v>
       </c>
-      <c r="B5" s="19">
+      <c r="B5" s="18">
         <f t="shared" si="1"/>
         <v>7</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="D5" s="4" t="s">
         <v>88</v>
@@ -1937,29 +1939,29 @@
         <v>17</v>
       </c>
       <c r="J5" s="3" t="s">
-        <v>13</v>
+        <v>262</v>
       </c>
       <c r="K5" s="3" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="L5" s="3" t="s">
-        <v>143</v>
+        <v>263</v>
       </c>
       <c r="M5" s="2" t="s">
-        <v>144</v>
+        <v>264</v>
       </c>
       <c r="N5" s="2" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="O5" s="5">
-        <v>0.32</v>
+        <v>0.36</v>
       </c>
       <c r="P5" s="5">
         <v>0.32</v>
       </c>
       <c r="Q5" s="6">
         <f t="shared" si="2"/>
-        <v>2.2400000000000002</v>
+        <v>2.52</v>
       </c>
       <c r="R5" s="6">
         <f t="shared" si="4"/>
@@ -1967,7 +1969,7 @@
       </c>
       <c r="S5" s="6">
         <f t="shared" si="3"/>
-        <v>2.2400000000000002</v>
+        <v>2.52</v>
       </c>
       <c r="T5" s="6">
         <f t="shared" si="5"/>
@@ -1976,11 +1978,11 @@
       <c r="U5" s="4"/>
       <c r="V5" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>7,399-9879-1-ND</v>
+        <v>7,BC3323-ND</v>
       </c>
       <c r="W5" s="4" t="str">
         <f t="shared" si="6"/>
-        <v>7,399-9879-1-ND</v>
+        <v>7,BC3323-ND</v>
       </c>
       <c r="X5" t="str">
         <f t="shared" si="7"/>
@@ -1992,15 +1994,15 @@
       </c>
       <c r="Z5" t="str">
         <f t="shared" si="9"/>
-        <v>C322C104M5R5TA7301 7</v>
+        <v>K104K15X7RF53H5 7</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="17" thickBot="1">
-      <c r="A6" s="19">
+      <c r="A6" s="18">
         <f>LEN(C6)-LEN(SUBSTITUTE(C6,",",""))+1</f>
         <v>1</v>
       </c>
-      <c r="B6" s="19">
+      <c r="B6" s="18">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
@@ -2014,7 +2016,7 @@
         <v>15</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="G6" s="3" t="s">
         <v>9</v>
@@ -2027,16 +2029,16 @@
         <v>13</v>
       </c>
       <c r="K6" s="3" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="L6" s="3" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="M6" s="2" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="N6" s="2" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="O6" s="5">
         <v>1.57</v>
@@ -2083,11 +2085,11 @@
       </c>
     </row>
     <row r="7" spans="1:26" ht="17" thickBot="1">
-      <c r="A7" s="19">
+      <c r="A7" s="18">
         <f t="shared" ref="A7:A9" si="10">LEN(C7)-LEN(SUBSTITUTE(C7,",",""))+1</f>
         <v>1</v>
       </c>
-      <c r="B7" s="19">
+      <c r="B7" s="18">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
@@ -2101,7 +2103,7 @@
         <v>16</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="G7" s="3" t="s">
         <v>12</v>
@@ -2114,16 +2116,16 @@
         <v>10</v>
       </c>
       <c r="K7" s="3" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="L7" s="3" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="M7" s="2" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="N7" s="2" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="O7" s="5">
         <v>0.62</v>
@@ -2170,25 +2172,25 @@
       </c>
     </row>
     <row r="8" spans="1:26" ht="17" thickBot="1">
-      <c r="A8" s="19">
+      <c r="A8" s="18">
         <f t="shared" si="10"/>
         <v>2</v>
       </c>
-      <c r="B8" s="19">
+      <c r="B8" s="18">
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="E8" s="3" t="s">
         <v>17</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="G8" s="3" t="s">
         <v>12</v>
@@ -2201,16 +2203,16 @@
         <v>13</v>
       </c>
       <c r="K8" s="3" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="L8" s="3" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="M8" s="2" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="N8" s="2" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="O8" s="5">
         <v>0.24</v>
@@ -2257,18 +2259,18 @@
       </c>
     </row>
     <row r="9" spans="1:26" ht="17" thickBot="1">
-      <c r="A9" s="19">
+      <c r="A9" s="18">
         <f t="shared" si="10"/>
         <v>3</v>
       </c>
-      <c r="B9" s="19">
+      <c r="B9" s="18">
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>225</v>
-      </c>
-      <c r="D9" s="23" t="s">
+        <v>223</v>
+      </c>
+      <c r="D9" s="22" t="s">
         <v>135</v>
       </c>
       <c r="E9" s="3" t="s">
@@ -2288,7 +2290,7 @@
         <v>13</v>
       </c>
       <c r="K9" s="3" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="L9" s="3" t="s">
         <v>140</v>
@@ -2297,7 +2299,7 @@
         <v>141</v>
       </c>
       <c r="N9" s="2" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="O9" s="5">
         <v>0.66</v>
@@ -2344,11 +2346,11 @@
       </c>
     </row>
     <row r="10" spans="1:26" ht="17" thickBot="1">
-      <c r="A10" s="19">
+      <c r="A10" s="18">
         <f>LEN(C10)-LEN(SUBSTITUTE(C10,",",""))+1</f>
         <v>1</v>
       </c>
-      <c r="B10" s="19">
+      <c r="B10" s="18">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
@@ -2373,7 +2375,7 @@
         <v>13</v>
       </c>
       <c r="K10" s="3" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="L10" s="3" t="s">
         <v>113</v>
@@ -2382,7 +2384,7 @@
         <v>112</v>
       </c>
       <c r="N10" s="2" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="O10" s="5">
         <v>0.25</v>
@@ -2429,8 +2431,8 @@
       </c>
     </row>
     <row r="11" spans="1:26" ht="17" thickBot="1">
-      <c r="A11" s="17"/>
-      <c r="B11" s="17"/>
+      <c r="A11" s="16"/>
+      <c r="B11" s="16"/>
       <c r="C11" s="4"/>
       <c r="D11" s="4"/>
       <c r="E11" s="3"/>
@@ -2468,11 +2470,11 @@
       </c>
     </row>
     <row r="12" spans="1:26" ht="17" thickBot="1">
-      <c r="A12" s="19">
+      <c r="A12" s="18">
         <f>LEN(C12)-LEN(SUBSTITUTE(C12,",",""))+1</f>
         <v>1</v>
       </c>
-      <c r="B12" s="19">
+      <c r="B12" s="18">
         <f t="shared" ref="B12:B15" si="11">LEN(D12)-LEN(SUBSTITUTE(D12,",",""))+1</f>
         <v>1</v>
       </c>
@@ -2499,7 +2501,7 @@
         <v>21</v>
       </c>
       <c r="K12" s="3" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="L12" s="7" t="s">
         <v>22</v>
@@ -2508,7 +2510,7 @@
         <v>23</v>
       </c>
       <c r="N12" s="2" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="O12" s="5">
         <v>0.34</v>
@@ -2554,20 +2556,20 @@
         <v>1N5919BG 1</v>
       </c>
     </row>
-    <row r="13" spans="1:26" ht="27" thickBot="1">
-      <c r="A13" s="19">
+    <row r="13" spans="1:26" ht="29" thickBot="1">
+      <c r="A13" s="18">
         <f>LEN(C13)-LEN(SUBSTITUTE(C13,",",""))+1</f>
         <v>2</v>
       </c>
-      <c r="B13" s="19">
+      <c r="B13" s="18">
         <f t="shared" si="11"/>
         <v>2</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="E13" s="3" t="s">
         <v>123</v>
@@ -2586,7 +2588,7 @@
         <v>26</v>
       </c>
       <c r="K13" s="3" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="L13" s="3" t="s">
         <v>24</v>
@@ -2595,7 +2597,7 @@
         <v>27</v>
       </c>
       <c r="N13" s="2" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="O13" s="5">
         <v>0.39</v>
@@ -2642,18 +2644,18 @@
       </c>
     </row>
     <row r="14" spans="1:26" ht="17" thickBot="1">
-      <c r="A14" s="19">
+      <c r="A14" s="18">
         <f>LEN(C14)-LEN(SUBSTITUTE(C14,",",""))+1</f>
         <v>8</v>
       </c>
-      <c r="B14" s="19">
+      <c r="B14" s="18">
         <f t="shared" si="11"/>
         <v>4</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>227</v>
-      </c>
-      <c r="D14" s="23" t="s">
+        <v>225</v>
+      </c>
+      <c r="D14" s="22" t="s">
         <v>131</v>
       </c>
       <c r="E14" s="3" t="s">
@@ -2669,16 +2671,16 @@
       <c r="I14" s="3"/>
       <c r="J14" s="3"/>
       <c r="K14" s="3" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="L14" s="3" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="M14" s="2" t="s">
         <v>97</v>
       </c>
       <c r="N14" s="2" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="O14" s="5">
         <v>0.47</v>
@@ -2724,19 +2726,19 @@
         <v>LTL-4221N 8</v>
       </c>
     </row>
-    <row r="15" spans="1:26" ht="27" thickBot="1">
-      <c r="A15" s="19">
+    <row r="15" spans="1:26" ht="29" thickBot="1">
+      <c r="A15" s="18">
         <f>LEN(C15)-LEN(SUBSTITUTE(C15,",",""))+1</f>
         <v>4</v>
       </c>
-      <c r="B15" s="19">
+      <c r="B15" s="18">
         <f t="shared" si="11"/>
         <v>2</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>228</v>
-      </c>
-      <c r="D15" s="23" t="s">
+        <v>226</v>
+      </c>
+      <c r="D15" s="22" t="s">
         <v>130</v>
       </c>
       <c r="E15" s="3" t="s">
@@ -2756,7 +2758,7 @@
         <v>26</v>
       </c>
       <c r="K15" s="3" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="L15" s="3" t="s">
         <v>31</v>
@@ -2765,7 +2767,7 @@
         <v>32</v>
       </c>
       <c r="N15" s="2" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="O15" s="5">
         <v>0.11</v>
@@ -2812,8 +2814,8 @@
       </c>
     </row>
     <row r="16" spans="1:26" ht="17" thickBot="1">
-      <c r="A16" s="17"/>
-      <c r="B16" s="17"/>
+      <c r="A16" s="16"/>
+      <c r="B16" s="16"/>
       <c r="C16" s="4"/>
       <c r="D16" s="4"/>
       <c r="E16" s="3"/>
@@ -2855,10 +2857,10 @@
       </c>
     </row>
     <row r="17" spans="1:26" ht="17" thickBot="1">
-      <c r="A17" s="19">
+      <c r="A17" s="18">
         <v>1</v>
       </c>
-      <c r="B17" s="19">
+      <c r="B17" s="18">
         <f t="shared" ref="B17" si="14">LEN(D17)-LEN(SUBSTITUTE(D17,",",""))+1</f>
         <v>1</v>
       </c>
@@ -2885,7 +2887,7 @@
         <v>36</v>
       </c>
       <c r="K17" s="3" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="L17" s="3" t="s">
         <v>37</v>
@@ -2894,7 +2896,7 @@
         <v>38</v>
       </c>
       <c r="N17" s="2" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="O17" s="5">
         <v>0.72</v>
@@ -2941,8 +2943,8 @@
       </c>
     </row>
     <row r="18" spans="1:26" ht="17" thickBot="1">
-      <c r="A18" s="17"/>
-      <c r="B18" s="17"/>
+      <c r="A18" s="16"/>
+      <c r="B18" s="16"/>
       <c r="C18" s="4"/>
       <c r="D18" s="4"/>
       <c r="E18" s="3"/>
@@ -2989,16 +2991,16 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="19" spans="1:26" ht="27" thickBot="1">
-      <c r="A19" s="19">
+    <row r="19" spans="1:26" ht="29" thickBot="1">
+      <c r="A19" s="18">
         <v>1</v>
       </c>
-      <c r="B19" s="19">
+      <c r="B19" s="18">
         <f t="shared" ref="B19" si="16">LEN(D19)-LEN(SUBSTITUTE(D19,",",""))+1</f>
         <v>1</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="D19" s="4" t="s">
         <v>107</v>
@@ -3016,7 +3018,7 @@
         <v>105</v>
       </c>
       <c r="K19" s="3" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="L19" s="3" t="s">
         <v>108</v>
@@ -3025,7 +3027,7 @@
         <v>104</v>
       </c>
       <c r="N19" s="2" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="O19" s="3">
         <v>0.40200000000000002</v>
@@ -3074,10 +3076,10 @@
       </c>
     </row>
     <row r="20" spans="1:26" ht="17" thickBot="1">
-      <c r="A20" s="19">
+      <c r="A20" s="18">
         <v>5</v>
       </c>
-      <c r="B20" s="19">
+      <c r="B20" s="18">
         <v>5</v>
       </c>
       <c r="C20" s="4" t="s">
@@ -3097,16 +3099,16 @@
       <c r="I20" s="3"/>
       <c r="J20" s="3"/>
       <c r="K20" s="3" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="L20" s="3" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="M20" s="2" t="s">
         <v>89</v>
       </c>
       <c r="N20" s="3" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="O20" s="5">
         <v>0.1</v>
@@ -3152,11 +3154,11 @@
         <v>969102-0000-DA 5</v>
       </c>
     </row>
-    <row r="21" spans="1:26" ht="27" thickBot="1">
-      <c r="A21" s="19">
+    <row r="21" spans="1:26" ht="29" thickBot="1">
+      <c r="A21" s="18">
         <v>4</v>
       </c>
-      <c r="B21" s="19">
+      <c r="B21" s="18">
         <v>4</v>
       </c>
       <c r="C21" s="4" t="s">
@@ -3180,21 +3182,21 @@
         <v>101</v>
       </c>
       <c r="K21" s="3" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="L21" s="3" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="M21" s="2" t="s">
         <v>100</v>
       </c>
       <c r="N21" s="2" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="O21" s="6">
         <v>0.56000000000000005</v>
       </c>
-      <c r="P21" s="26">
+      <c r="P21" s="25">
         <v>2.95</v>
       </c>
       <c r="Q21" s="6">
@@ -3214,7 +3216,7 @@
         <v>11.8</v>
       </c>
       <c r="U21" s="4" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="V21" s="4" t="str">
         <f t="shared" si="0"/>
@@ -3237,24 +3239,24 @@
         <v>PREC040SAAN-RC.. 4</v>
       </c>
     </row>
-    <row r="22" spans="1:26" ht="40" thickBot="1">
-      <c r="A22" s="19">
+    <row r="22" spans="1:26" ht="43" thickBot="1">
+      <c r="A22" s="18">
         <v>1</v>
       </c>
-      <c r="B22" s="19">
+      <c r="B22" s="18">
         <v>1</v>
       </c>
-      <c r="C22" s="3" t="s">
-        <v>177</v>
-      </c>
-      <c r="D22" s="3" t="s">
-        <v>177</v>
+      <c r="C22" s="4" t="s">
+        <v>175</v>
+      </c>
+      <c r="D22" s="4" t="s">
+        <v>175</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="F22" s="3" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="G22" s="3"/>
       <c r="H22" s="3"/>
@@ -3262,19 +3264,19 @@
         <v>1</v>
       </c>
       <c r="J22" s="3" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="K22" s="3" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="L22" s="3" t="s">
-        <v>176</v>
-      </c>
-      <c r="M22" s="15" t="s">
-        <v>172</v>
+        <v>174</v>
+      </c>
+      <c r="M22" s="2" t="s">
+        <v>170</v>
       </c>
       <c r="N22" s="2" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="O22" s="6">
         <v>1.1299999999999999</v>
@@ -3321,8 +3323,8 @@
       </c>
     </row>
     <row r="23" spans="1:26" ht="17" thickBot="1">
-      <c r="A23" s="17"/>
-      <c r="B23" s="17"/>
+      <c r="A23" s="16"/>
+      <c r="B23" s="16"/>
       <c r="C23" s="4"/>
       <c r="D23" s="4"/>
       <c r="E23" s="3"/>
@@ -3363,26 +3365,26 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="24" spans="1:26" ht="27" thickBot="1">
-      <c r="A24" s="19">
+    <row r="24" spans="1:26" ht="29" thickBot="1">
+      <c r="A24" s="18">
         <f>LEN(C24)-LEN(SUBSTITUTE(C24,",",""))+1</f>
         <v>8</v>
       </c>
-      <c r="B24" s="19">
+      <c r="B24" s="18">
         <f t="shared" ref="B24" si="20">LEN(D24)-LEN(SUBSTITUTE(D24,",",""))+1</f>
         <v>6</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>230</v>
-      </c>
-      <c r="D24" s="23" t="s">
+        <v>228</v>
+      </c>
+      <c r="D24" s="22" t="s">
         <v>129</v>
       </c>
       <c r="E24" s="3" t="s">
         <v>117</v>
       </c>
       <c r="F24" s="3" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="G24" s="3" t="s">
         <v>66</v>
@@ -3395,16 +3397,16 @@
         <v>40</v>
       </c>
       <c r="K24" s="3" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="L24" s="3" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="M24" s="2" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="N24" s="2" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="O24" s="6">
         <v>1.51</v>
@@ -3451,8 +3453,8 @@
       </c>
     </row>
     <row r="25" spans="1:26" ht="17" thickBot="1">
-      <c r="A25" s="17"/>
-      <c r="B25" s="17"/>
+      <c r="A25" s="16"/>
+      <c r="B25" s="16"/>
       <c r="C25" s="4"/>
       <c r="D25" s="4"/>
       <c r="E25" s="3"/>
@@ -3490,19 +3492,19 @@
       </c>
     </row>
     <row r="26" spans="1:26" ht="17" thickBot="1">
-      <c r="A26" s="19">
+      <c r="A26" s="18">
         <f>LEN(C26)-LEN(SUBSTITUTE(C26,",",""))+1</f>
         <v>1</v>
       </c>
-      <c r="B26" s="19">
+      <c r="B26" s="18">
         <f t="shared" ref="A26:B31" si="21">LEN(D26)-LEN(SUBSTITUTE(D26,",",""))+1</f>
         <v>1</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="D26" s="4" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="E26" s="3" t="s">
         <v>41</v>
@@ -3519,16 +3521,16 @@
         <v>43</v>
       </c>
       <c r="K26" s="3" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="L26" s="3" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="M26" s="2" t="s">
         <v>44</v>
       </c>
       <c r="N26" s="2" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="O26" s="5">
         <v>0.08</v>
@@ -3574,20 +3576,20 @@
         <v>MFR-25FBF52-10K 1</v>
       </c>
     </row>
-    <row r="27" spans="1:26" ht="27" thickBot="1">
-      <c r="A27" s="19">
+    <row r="27" spans="1:26" ht="29" thickBot="1">
+      <c r="A27" s="18">
         <f>LEN(C27)-LEN(SUBSTITUTE(C27,",",""))+1</f>
         <v>17</v>
       </c>
-      <c r="B27" s="19">
+      <c r="B27" s="18">
         <f t="shared" si="21"/>
         <v>13</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>248</v>
-      </c>
-      <c r="D27" s="23" t="s">
-        <v>249</v>
+        <v>246</v>
+      </c>
+      <c r="D27" s="22" t="s">
+        <v>247</v>
       </c>
       <c r="E27" s="3" t="s">
         <v>45</v>
@@ -3604,16 +3606,16 @@
         <v>43</v>
       </c>
       <c r="K27" s="3" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="L27" s="3" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="M27" s="2" t="s">
         <v>47</v>
       </c>
       <c r="N27" s="2" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="O27" s="5">
         <v>0.06</v>
@@ -3660,19 +3662,19 @@
       </c>
     </row>
     <row r="28" spans="1:26" ht="17" thickBot="1">
-      <c r="A28" s="19">
+      <c r="A28" s="18">
         <f>LEN(C28)-LEN(SUBSTITUTE(C28,",",""))+1</f>
         <v>4</v>
       </c>
-      <c r="B28" s="19">
+      <c r="B28" s="18">
         <f t="shared" si="21"/>
         <v>2</v>
       </c>
       <c r="C28" s="12" t="s">
+        <v>248</v>
+      </c>
+      <c r="D28" s="23" t="s">
         <v>250</v>
-      </c>
-      <c r="D28" s="24" t="s">
-        <v>252</v>
       </c>
       <c r="E28" s="13">
         <v>680</v>
@@ -3687,16 +3689,16 @@
         <v>138</v>
       </c>
       <c r="K28" s="13" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="L28" s="7" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="M28" s="2" t="s">
         <v>136</v>
       </c>
       <c r="N28" s="2" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="O28" s="14">
         <v>0.22</v>
@@ -3744,20 +3746,20 @@
         <v>1622545-1 4</v>
       </c>
     </row>
-    <row r="29" spans="1:26" ht="27" thickBot="1">
-      <c r="A29" s="19">
+    <row r="29" spans="1:26" ht="29" thickBot="1">
+      <c r="A29" s="18">
         <f>LEN(C29)-LEN(SUBSTITUTE(C29,",",""))+1</f>
         <v>6</v>
       </c>
-      <c r="B29" s="19">
+      <c r="B29" s="18">
         <f t="shared" si="21"/>
         <v>6</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="D29" s="4" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="E29" s="3">
         <v>470</v>
@@ -3774,7 +3776,7 @@
         <v>49</v>
       </c>
       <c r="K29" s="3" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="L29" s="7" t="s">
         <v>50</v>
@@ -3783,7 +3785,7 @@
         <v>51</v>
       </c>
       <c r="N29" s="2" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="O29" s="5">
         <v>0.11</v>
@@ -3829,26 +3831,26 @@
         <v>RNF14FTD470R 6</v>
       </c>
     </row>
-    <row r="30" spans="1:26" ht="27" thickBot="1">
-      <c r="A30" s="19">
+    <row r="30" spans="1:26" ht="29" thickBot="1">
+      <c r="A30" s="18">
         <f t="shared" si="21"/>
         <v>7</v>
       </c>
-      <c r="B30" s="19">
+      <c r="B30" s="18">
         <f t="shared" si="21"/>
         <v>5</v>
       </c>
       <c r="C30" s="4" t="s">
+        <v>249</v>
+      </c>
+      <c r="D30" s="4" t="s">
         <v>251</v>
       </c>
-      <c r="D30" s="4" t="s">
-        <v>253</v>
-      </c>
       <c r="E30" s="3" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="F30" s="3" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="G30" s="3" t="s">
         <v>52</v>
@@ -3861,16 +3863,16 @@
         <v>43</v>
       </c>
       <c r="K30" s="3" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="L30" s="3" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="M30" s="2" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="N30" s="2" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="O30" s="5">
         <v>0.14000000000000001</v>
@@ -3917,10 +3919,10 @@
       </c>
     </row>
     <row r="31" spans="1:26" ht="17" thickBot="1">
-      <c r="A31" s="19">
+      <c r="A31" s="18">
         <v>1</v>
       </c>
-      <c r="B31" s="19">
+      <c r="B31" s="18">
         <f t="shared" si="21"/>
         <v>1</v>
       </c>
@@ -3945,7 +3947,7 @@
         <v>43</v>
       </c>
       <c r="K31" s="3" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="L31" s="3" t="s">
         <v>54</v>
@@ -3954,7 +3956,7 @@
         <v>55</v>
       </c>
       <c r="N31" s="2" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="O31" s="5">
         <v>0.46</v>
@@ -4003,18 +4005,18 @@
       </c>
     </row>
     <row r="32" spans="1:26" ht="17" thickBot="1">
-      <c r="A32" s="19">
+      <c r="A32" s="18">
         <f t="shared" ref="A32:A33" si="25">LEN(C32)-LEN(SUBSTITUTE(C32,",",""))+1</f>
         <v>12</v>
       </c>
-      <c r="B32" s="19">
+      <c r="B32" s="18">
         <f>LEN(D32)-LEN(SUBSTITUTE(D32,",",""))+1</f>
         <v>8</v>
       </c>
       <c r="C32" s="4" t="s">
-        <v>232</v>
-      </c>
-      <c r="D32" s="23" t="s">
+        <v>230</v>
+      </c>
+      <c r="D32" s="22" t="s">
         <v>134</v>
       </c>
       <c r="E32" s="3" t="s">
@@ -4032,16 +4034,16 @@
         <v>43</v>
       </c>
       <c r="K32" s="3" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="L32" s="3" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="M32" s="2" t="s">
         <v>58</v>
       </c>
       <c r="N32" s="2" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="O32" s="5">
         <v>0.1</v>
@@ -4088,18 +4090,18 @@
       </c>
     </row>
     <row r="33" spans="1:26" ht="17" thickBot="1">
-      <c r="A33" s="19">
+      <c r="A33" s="18">
         <f t="shared" si="25"/>
         <v>4</v>
       </c>
-      <c r="B33" s="19">
+      <c r="B33" s="18">
         <f>LEN(D33)-LEN(SUBSTITUTE(D33,",",""))+1</f>
         <v>2</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>233</v>
-      </c>
-      <c r="D33" s="23" t="s">
+        <v>231</v>
+      </c>
+      <c r="D33" s="22" t="s">
         <v>132</v>
       </c>
       <c r="E33" s="3">
@@ -4117,7 +4119,7 @@
         <v>43</v>
       </c>
       <c r="K33" s="3" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="L33" s="3" t="s">
         <v>60</v>
@@ -4126,7 +4128,7 @@
         <v>61</v>
       </c>
       <c r="N33" s="2" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="O33" s="5">
         <v>0.27</v>
@@ -4173,8 +4175,8 @@
       </c>
     </row>
     <row r="34" spans="1:26" ht="17" thickBot="1">
-      <c r="A34" s="17"/>
-      <c r="B34" s="17"/>
+      <c r="A34" s="16"/>
+      <c r="B34" s="16"/>
       <c r="C34" s="4"/>
       <c r="D34" s="4"/>
       <c r="E34" s="3"/>
@@ -4211,11 +4213,11 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="35" spans="1:26" ht="27" thickBot="1">
-      <c r="A35" s="19">
+    <row r="35" spans="1:26" ht="29" thickBot="1">
+      <c r="A35" s="18">
         <v>1</v>
       </c>
-      <c r="B35" s="19">
+      <c r="B35" s="18">
         <f t="shared" ref="B35:B37" si="26">LEN(D35)-LEN(SUBSTITUTE(D35,",",""))+1</f>
         <v>1</v>
       </c>
@@ -4242,7 +4244,7 @@
         <v>67</v>
       </c>
       <c r="K35" s="3" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="L35" s="3" t="s">
         <v>64</v>
@@ -4251,7 +4253,7 @@
         <v>64</v>
       </c>
       <c r="N35" s="2" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="O35" s="5">
         <v>1.68</v>
@@ -4297,11 +4299,11 @@
         <v>LM2940T-5.0/NOPB 1</v>
       </c>
     </row>
-    <row r="36" spans="1:26" ht="27" thickBot="1">
-      <c r="A36" s="19">
+    <row r="36" spans="1:26" ht="29" thickBot="1">
+      <c r="A36" s="18">
         <v>1</v>
       </c>
-      <c r="B36" s="19">
+      <c r="B36" s="18">
         <f t="shared" si="26"/>
         <v>1</v>
       </c>
@@ -4329,13 +4331,13 @@
       </c>
       <c r="K36" s="3"/>
       <c r="L36" s="3" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="M36" s="2" t="s">
         <v>80</v>
       </c>
       <c r="N36" s="2" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="O36" s="6">
         <v>15.41</v>
@@ -4381,16 +4383,16 @@
         <v>MPX4250AP 1</v>
       </c>
     </row>
-    <row r="37" spans="1:26" ht="27" thickBot="1">
-      <c r="A37" s="19">
+    <row r="37" spans="1:26" ht="29" thickBot="1">
+      <c r="A37" s="18">
         <v>2</v>
       </c>
-      <c r="B37" s="19">
+      <c r="B37" s="18">
         <f t="shared" si="26"/>
         <v>1</v>
       </c>
       <c r="C37" s="12" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="D37" s="12" t="s">
         <v>133</v>
@@ -4412,7 +4414,7 @@
         <v>68</v>
       </c>
       <c r="K37" s="13" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="L37" s="13" t="s">
         <v>124</v>
@@ -4421,12 +4423,12 @@
         <v>127</v>
       </c>
       <c r="N37" s="13" t="s">
-        <v>186</v>
-      </c>
-      <c r="O37" s="21">
+        <v>184</v>
+      </c>
+      <c r="O37" s="20">
         <v>2.92</v>
       </c>
-      <c r="P37" s="21">
+      <c r="P37" s="20">
         <v>2.92</v>
       </c>
       <c r="Q37" s="6">
@@ -4468,23 +4470,23 @@
       </c>
     </row>
     <row r="38" spans="1:26" ht="17" thickBot="1">
-      <c r="A38" s="19">
+      <c r="A38" s="18">
         <v>1</v>
       </c>
-      <c r="B38" s="28">
+      <c r="B38" s="27">
         <v>1</v>
       </c>
       <c r="C38" s="12" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="D38" s="12" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="E38" s="13" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="F38" s="3" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="G38" s="3" t="s">
         <v>126</v>
@@ -4494,19 +4496,19 @@
         <v>1</v>
       </c>
       <c r="J38" s="13" t="s">
+        <v>218</v>
+      </c>
+      <c r="K38" s="26" t="s">
+        <v>158</v>
+      </c>
+      <c r="L38" s="13" t="s">
+        <v>216</v>
+      </c>
+      <c r="M38" s="13" t="s">
+        <v>219</v>
+      </c>
+      <c r="N38" s="2" t="s">
         <v>220</v>
-      </c>
-      <c r="K38" s="27" t="s">
-        <v>160</v>
-      </c>
-      <c r="L38" s="13" t="s">
-        <v>218</v>
-      </c>
-      <c r="M38" s="13" t="s">
-        <v>221</v>
-      </c>
-      <c r="N38" s="2" t="s">
-        <v>222</v>
       </c>
       <c r="O38" s="6">
         <v>2.4</v>
@@ -4553,37 +4555,37 @@
       </c>
     </row>
     <row r="39" spans="1:26" ht="17" thickBot="1">
-      <c r="A39" s="19">
+      <c r="A39" s="18">
         <v>3</v>
       </c>
-      <c r="B39" s="19">
+      <c r="B39" s="27">
         <v>2</v>
       </c>
-      <c r="C39" s="15" t="s">
+      <c r="C39" s="12" t="s">
         <v>86</v>
       </c>
-      <c r="D39" s="15" t="s">
+      <c r="D39" s="12" t="s">
         <v>86</v>
       </c>
-      <c r="E39" s="3" t="s">
+      <c r="E39" s="13" t="s">
         <v>119</v>
       </c>
       <c r="F39" s="3"/>
       <c r="G39" s="3"/>
-      <c r="H39" s="3"/>
-      <c r="I39" s="3"/>
-      <c r="J39" s="3"/>
-      <c r="K39" s="3" t="s">
-        <v>160</v>
-      </c>
-      <c r="L39" s="3" t="s">
+      <c r="H39" s="13"/>
+      <c r="I39" s="13"/>
+      <c r="J39" s="13"/>
+      <c r="K39" s="26" t="s">
+        <v>158</v>
+      </c>
+      <c r="L39" s="13" t="s">
         <v>85</v>
       </c>
-      <c r="M39" s="2" t="s">
+      <c r="M39" s="13" t="s">
         <v>84</v>
       </c>
       <c r="N39" s="2" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="O39" s="6">
         <v>0.5</v>
@@ -4630,8 +4632,8 @@
       </c>
     </row>
     <row r="40" spans="1:26" ht="17" thickBot="1">
-      <c r="A40" s="17"/>
-      <c r="B40" s="17"/>
+      <c r="A40" s="16"/>
+      <c r="B40" s="16"/>
       <c r="C40" s="4"/>
       <c r="D40" s="4"/>
       <c r="E40" s="3"/>
@@ -4664,18 +4666,18 @@
         <v/>
       </c>
     </row>
-    <row r="41" spans="1:26" ht="27" thickBot="1">
-      <c r="A41" s="17">
+    <row r="41" spans="1:26" ht="29" thickBot="1">
+      <c r="A41" s="16">
         <v>1</v>
       </c>
-      <c r="B41" s="17">
+      <c r="B41" s="16">
         <v>1</v>
       </c>
       <c r="C41" s="4" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="D41" s="4" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="E41" s="3"/>
       <c r="F41" s="3"/>
@@ -4685,17 +4687,17 @@
         <v>1</v>
       </c>
       <c r="J41" s="3" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="K41" s="3"/>
       <c r="L41" s="3" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="M41" s="13" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="N41" s="13" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="O41" s="6">
         <v>15.33</v>
@@ -4734,8 +4736,8 @@
       </c>
     </row>
     <row r="42" spans="1:26" ht="17" thickBot="1">
-      <c r="A42" s="17"/>
-      <c r="B42" s="17"/>
+      <c r="A42" s="16"/>
+      <c r="B42" s="16"/>
       <c r="C42" s="4"/>
       <c r="D42" s="4"/>
       <c r="E42" s="3"/>
@@ -4765,8 +4767,8 @@
       </c>
     </row>
     <row r="43" spans="1:26" ht="17" thickBot="1">
-      <c r="A43" s="17"/>
-      <c r="B43" s="17"/>
+      <c r="A43" s="16"/>
+      <c r="B43" s="16"/>
       <c r="C43" s="4" t="s">
         <v>71</v>
       </c>
@@ -4776,7 +4778,7 @@
       <c r="E43" s="3"/>
       <c r="F43" s="3"/>
       <c r="G43" s="3"/>
-      <c r="H43" s="22"/>
+      <c r="H43" s="21"/>
       <c r="I43" s="8"/>
       <c r="J43" s="4"/>
       <c r="K43" s="8"/>
@@ -4800,15 +4802,15 @@
       </c>
     </row>
     <row r="44" spans="1:26" ht="17" thickBot="1">
-      <c r="A44" s="17">
+      <c r="A44" s="16">
         <v>1</v>
       </c>
-      <c r="B44" s="17"/>
+      <c r="B44" s="16"/>
       <c r="C44" s="4" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="D44" s="4" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="E44" s="3" t="s">
         <v>72</v>
@@ -4852,10 +4854,10 @@
       <c r="W44" s="4"/>
     </row>
     <row r="45" spans="1:26" ht="17" thickBot="1">
-      <c r="A45" s="17">
+      <c r="A45" s="16">
         <v>1</v>
       </c>
-      <c r="B45" s="17"/>
+      <c r="B45" s="16"/>
       <c r="C45" s="4" t="s">
         <v>92</v>
       </c>
@@ -4887,29 +4889,29 @@
       </c>
     </row>
     <row r="46" spans="1:26" ht="17" thickBot="1">
-      <c r="A46" s="17"/>
-      <c r="B46" s="17"/>
+      <c r="A46" s="16"/>
+      <c r="B46" s="16"/>
       <c r="C46" s="4"/>
       <c r="D46" s="4"/>
       <c r="E46" s="3"/>
       <c r="F46" s="3"/>
       <c r="G46" s="3"/>
-      <c r="H46" s="22"/>
+      <c r="H46" s="21"/>
       <c r="I46" s="8"/>
       <c r="J46" s="4"/>
       <c r="K46" s="8"/>
-      <c r="L46" s="29" t="s">
+      <c r="L46" s="28" t="s">
         <v>74</v>
       </c>
-      <c r="M46" s="30"/>
-      <c r="N46" s="25"/>
+      <c r="M46" s="29"/>
+      <c r="N46" s="24"/>
       <c r="O46" s="1" t="s">
         <v>69</v>
       </c>
       <c r="P46" s="1"/>
       <c r="Q46" s="11">
         <f>SUM(Q2:Q45)</f>
-        <v>98.712000000000003</v>
+        <v>98.992000000000004</v>
       </c>
       <c r="R46" s="11">
         <f>SUM(R2:R45)</f>
@@ -4917,7 +4919,7 @@
       </c>
       <c r="S46" s="11">
         <f>SUM(S2:S45)</f>
-        <v>72.612000000000009</v>
+        <v>72.89200000000001</v>
       </c>
       <c r="T46" s="11">
         <f>SUM(T2:T45)</f>
@@ -4946,7 +4948,7 @@
     <hyperlink ref="M32" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
   </hyperlinks>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" scale="27" orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <pageSetup paperSize="9" scale="62" orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <legacyDrawing r:id="rId12"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add design files for v0.4.4b board
</commit_message>
<xml_diff>
--- a/reference/hardware/v0.4/BOMs/v0.4.3_bom.xlsx
+++ b/reference/hardware/v0.4/BOMs/v0.4.3_bom.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11110"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10113"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/josh/Documents/Arduino/speeduino/reference/hardware/v0.4/BOMs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F0AFFD5-2611-D043-902D-0E690169F52E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1226EEB7-EB76-1645-891B-456F9204BC1C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16100" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
@@ -1117,7 +1119,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1142,9 +1144,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -1203,6 +1202,12 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="54">
@@ -1602,13 +1607,13 @@
   <dimension ref="A1:Z46"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="113" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="J41" sqref="J41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="1" width="18.83203125" style="17" customWidth="1"/>
-    <col min="2" max="2" width="18.83203125" style="17" hidden="1" customWidth="1"/>
+    <col min="1" max="1" width="18.83203125" style="16" customWidth="1"/>
+    <col min="2" max="2" width="18.83203125" style="16" hidden="1" customWidth="1"/>
     <col min="3" max="3" width="46.6640625" customWidth="1"/>
     <col min="4" max="4" width="46.6640625" hidden="1" customWidth="1"/>
     <col min="5" max="5" width="15" customWidth="1"/>
@@ -1625,10 +1630,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="29" thickBot="1">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="14" t="s">
         <v>160</v>
       </c>
-      <c r="B1" s="15" t="s">
+      <c r="B1" s="14" t="s">
         <v>161</v>
       </c>
       <c r="C1" s="1" t="s">
@@ -1661,7 +1666,7 @@
       <c r="L1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="M1" s="29" t="s">
         <v>6</v>
       </c>
       <c r="N1" s="1" t="s">
@@ -1688,22 +1693,22 @@
       <c r="U1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="V1" s="19" t="s">
+      <c r="V1" s="18" t="s">
         <v>176</v>
       </c>
-      <c r="W1" s="19" t="s">
+      <c r="W1" s="18" t="s">
         <v>177</v>
       </c>
-      <c r="X1" s="19" t="s">
+      <c r="X1" s="18" t="s">
         <v>120</v>
       </c>
-      <c r="Y1" s="19" t="s">
+      <c r="Y1" s="18" t="s">
         <v>178</v>
       </c>
     </row>
     <row r="2" spans="1:26" ht="17" thickBot="1">
-      <c r="A2" s="16"/>
-      <c r="B2" s="16"/>
+      <c r="A2" s="15"/>
+      <c r="B2" s="15"/>
       <c r="C2" s="4"/>
       <c r="D2" s="4"/>
       <c r="E2" s="3"/>
@@ -1714,7 +1719,7 @@
       <c r="J2" s="3"/>
       <c r="K2" s="3"/>
       <c r="L2" s="3"/>
-      <c r="M2" s="3"/>
+      <c r="M2" s="12"/>
       <c r="N2" s="3"/>
       <c r="O2" s="3"/>
       <c r="P2" s="3"/>
@@ -1737,11 +1742,11 @@
       </c>
     </row>
     <row r="3" spans="1:26" ht="17" thickBot="1">
-      <c r="A3" s="18">
+      <c r="A3" s="17">
         <f>LEN(C3)-LEN(SUBSTITUTE(C3,",",""))+1</f>
         <v>1</v>
       </c>
-      <c r="B3" s="18">
+      <c r="B3" s="17">
         <f t="shared" ref="B3:B10" si="1">LEN(D3)-LEN(SUBSTITUTE(D3,",",""))+1</f>
         <v>1</v>
       </c>
@@ -1773,7 +1778,7 @@
       <c r="L3" s="3" t="s">
         <v>145</v>
       </c>
-      <c r="M3" s="2" t="s">
+      <c r="M3" s="30" t="s">
         <v>146</v>
       </c>
       <c r="N3" s="2" t="s">
@@ -1824,11 +1829,11 @@
       </c>
     </row>
     <row r="4" spans="1:26" ht="17" thickBot="1">
-      <c r="A4" s="18">
+      <c r="A4" s="17">
         <f>LEN(C4)-LEN(SUBSTITUTE(C4,",",""))+1</f>
         <v>6</v>
       </c>
-      <c r="B4" s="18">
+      <c r="B4" s="17">
         <f t="shared" si="1"/>
         <v>6</v>
       </c>
@@ -1860,7 +1865,7 @@
       <c r="L4" s="3" t="s">
         <v>252</v>
       </c>
-      <c r="M4" s="2" t="s">
+      <c r="M4" s="30" t="s">
         <v>253</v>
       </c>
       <c r="N4" s="2" t="s">
@@ -1911,11 +1916,11 @@
       </c>
     </row>
     <row r="5" spans="1:26" ht="17" thickBot="1">
-      <c r="A5" s="18">
+      <c r="A5" s="17">
         <f>LEN(C5)-LEN(SUBSTITUTE(C5,",",""))+1</f>
         <v>7</v>
       </c>
-      <c r="B5" s="18">
+      <c r="B5" s="17">
         <f t="shared" si="1"/>
         <v>7</v>
       </c>
@@ -1947,7 +1952,7 @@
       <c r="L5" s="3" t="s">
         <v>263</v>
       </c>
-      <c r="M5" s="2" t="s">
+      <c r="M5" s="30" t="s">
         <v>264</v>
       </c>
       <c r="N5" s="2" t="s">
@@ -1998,11 +2003,11 @@
       </c>
     </row>
     <row r="6" spans="1:26" ht="17" thickBot="1">
-      <c r="A6" s="18">
+      <c r="A6" s="17">
         <f>LEN(C6)-LEN(SUBSTITUTE(C6,",",""))+1</f>
         <v>1</v>
       </c>
-      <c r="B6" s="18">
+      <c r="B6" s="17">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
@@ -2034,7 +2039,7 @@
       <c r="L6" s="3" t="s">
         <v>148</v>
       </c>
-      <c r="M6" s="2" t="s">
+      <c r="M6" s="30" t="s">
         <v>149</v>
       </c>
       <c r="N6" s="2" t="s">
@@ -2085,11 +2090,11 @@
       </c>
     </row>
     <row r="7" spans="1:26" ht="17" thickBot="1">
-      <c r="A7" s="18">
+      <c r="A7" s="17">
         <f t="shared" ref="A7:A9" si="10">LEN(C7)-LEN(SUBSTITUTE(C7,",",""))+1</f>
         <v>1</v>
       </c>
-      <c r="B7" s="18">
+      <c r="B7" s="17">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
@@ -2121,7 +2126,7 @@
       <c r="L7" s="3" t="s">
         <v>150</v>
       </c>
-      <c r="M7" s="2" t="s">
+      <c r="M7" s="30" t="s">
         <v>151</v>
       </c>
       <c r="N7" s="2" t="s">
@@ -2172,11 +2177,11 @@
       </c>
     </row>
     <row r="8" spans="1:26" ht="17" thickBot="1">
-      <c r="A8" s="18">
+      <c r="A8" s="17">
         <f t="shared" si="10"/>
         <v>2</v>
       </c>
-      <c r="B8" s="18">
+      <c r="B8" s="17">
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
@@ -2208,7 +2213,7 @@
       <c r="L8" s="3" t="s">
         <v>154</v>
       </c>
-      <c r="M8" s="2" t="s">
+      <c r="M8" s="30" t="s">
         <v>155</v>
       </c>
       <c r="N8" s="2" t="s">
@@ -2259,18 +2264,18 @@
       </c>
     </row>
     <row r="9" spans="1:26" ht="17" thickBot="1">
-      <c r="A9" s="18">
+      <c r="A9" s="17">
         <f t="shared" si="10"/>
         <v>3</v>
       </c>
-      <c r="B9" s="18">
+      <c r="B9" s="17">
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="C9" s="4" t="s">
         <v>223</v>
       </c>
-      <c r="D9" s="22" t="s">
+      <c r="D9" s="21" t="s">
         <v>135</v>
       </c>
       <c r="E9" s="3" t="s">
@@ -2295,7 +2300,7 @@
       <c r="L9" s="3" t="s">
         <v>140</v>
       </c>
-      <c r="M9" s="2" t="s">
+      <c r="M9" s="30" t="s">
         <v>141</v>
       </c>
       <c r="N9" s="2" t="s">
@@ -2346,11 +2351,11 @@
       </c>
     </row>
     <row r="10" spans="1:26" ht="17" thickBot="1">
-      <c r="A10" s="18">
+      <c r="A10" s="17">
         <f>LEN(C10)-LEN(SUBSTITUTE(C10,",",""))+1</f>
         <v>1</v>
       </c>
-      <c r="B10" s="18">
+      <c r="B10" s="17">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
@@ -2380,7 +2385,7 @@
       <c r="L10" s="3" t="s">
         <v>113</v>
       </c>
-      <c r="M10" s="2" t="s">
+      <c r="M10" s="30" t="s">
         <v>112</v>
       </c>
       <c r="N10" s="2" t="s">
@@ -2431,8 +2436,8 @@
       </c>
     </row>
     <row r="11" spans="1:26" ht="17" thickBot="1">
-      <c r="A11" s="16"/>
-      <c r="B11" s="16"/>
+      <c r="A11" s="15"/>
+      <c r="B11" s="15"/>
       <c r="C11" s="4"/>
       <c r="D11" s="4"/>
       <c r="E11" s="3"/>
@@ -2443,7 +2448,7 @@
       <c r="J11" s="3"/>
       <c r="K11" s="3"/>
       <c r="L11" s="3"/>
-      <c r="M11" s="2"/>
+      <c r="M11" s="30"/>
       <c r="N11" s="2"/>
       <c r="O11" s="3"/>
       <c r="P11" s="3"/>
@@ -2469,12 +2474,12 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="12" spans="1:26" ht="17" thickBot="1">
-      <c r="A12" s="18">
+    <row r="12" spans="1:26" ht="29" thickBot="1">
+      <c r="A12" s="17">
         <f>LEN(C12)-LEN(SUBSTITUTE(C12,",",""))+1</f>
         <v>1</v>
       </c>
-      <c r="B12" s="18">
+      <c r="B12" s="17">
         <f t="shared" ref="B12:B15" si="11">LEN(D12)-LEN(SUBSTITUTE(D12,",",""))+1</f>
         <v>1</v>
       </c>
@@ -2503,10 +2508,10 @@
       <c r="K12" s="3" t="s">
         <v>158</v>
       </c>
-      <c r="L12" s="7" t="s">
+      <c r="L12" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="M12" s="2" t="s">
+      <c r="M12" s="30" t="s">
         <v>23</v>
       </c>
       <c r="N12" s="2" t="s">
@@ -2557,11 +2562,11 @@
       </c>
     </row>
     <row r="13" spans="1:26" ht="29" thickBot="1">
-      <c r="A13" s="18">
+      <c r="A13" s="17">
         <f>LEN(C13)-LEN(SUBSTITUTE(C13,",",""))+1</f>
         <v>2</v>
       </c>
-      <c r="B13" s="18">
+      <c r="B13" s="17">
         <f t="shared" si="11"/>
         <v>2</v>
       </c>
@@ -2593,7 +2598,7 @@
       <c r="L13" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="M13" s="2" t="s">
+      <c r="M13" s="30" t="s">
         <v>27</v>
       </c>
       <c r="N13" s="2" t="s">
@@ -2644,18 +2649,18 @@
       </c>
     </row>
     <row r="14" spans="1:26" ht="17" thickBot="1">
-      <c r="A14" s="18">
+      <c r="A14" s="17">
         <f>LEN(C14)-LEN(SUBSTITUTE(C14,",",""))+1</f>
         <v>8</v>
       </c>
-      <c r="B14" s="18">
+      <c r="B14" s="17">
         <f t="shared" si="11"/>
         <v>4</v>
       </c>
       <c r="C14" s="4" t="s">
         <v>225</v>
       </c>
-      <c r="D14" s="22" t="s">
+      <c r="D14" s="21" t="s">
         <v>131</v>
       </c>
       <c r="E14" s="3" t="s">
@@ -2676,7 +2681,7 @@
       <c r="L14" s="3" t="s">
         <v>234</v>
       </c>
-      <c r="M14" s="2" t="s">
+      <c r="M14" s="30" t="s">
         <v>97</v>
       </c>
       <c r="N14" s="2" t="s">
@@ -2727,18 +2732,18 @@
       </c>
     </row>
     <row r="15" spans="1:26" ht="29" thickBot="1">
-      <c r="A15" s="18">
+      <c r="A15" s="17">
         <f>LEN(C15)-LEN(SUBSTITUTE(C15,",",""))+1</f>
         <v>4</v>
       </c>
-      <c r="B15" s="18">
+      <c r="B15" s="17">
         <f t="shared" si="11"/>
         <v>2</v>
       </c>
       <c r="C15" s="4" t="s">
         <v>226</v>
       </c>
-      <c r="D15" s="22" t="s">
+      <c r="D15" s="21" t="s">
         <v>130</v>
       </c>
       <c r="E15" s="3" t="s">
@@ -2763,7 +2768,7 @@
       <c r="L15" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="M15" s="2" t="s">
+      <c r="M15" s="30" t="s">
         <v>32</v>
       </c>
       <c r="N15" s="2" t="s">
@@ -2814,8 +2819,8 @@
       </c>
     </row>
     <row r="16" spans="1:26" ht="17" thickBot="1">
-      <c r="A16" s="16"/>
-      <c r="B16" s="16"/>
+      <c r="A16" s="15"/>
+      <c r="B16" s="15"/>
       <c r="C16" s="4"/>
       <c r="D16" s="4"/>
       <c r="E16" s="3"/>
@@ -2826,7 +2831,7 @@
       <c r="J16" s="3"/>
       <c r="K16" s="3"/>
       <c r="L16" s="3"/>
-      <c r="M16" s="2"/>
+      <c r="M16" s="30"/>
       <c r="N16" s="2"/>
       <c r="O16" s="3"/>
       <c r="P16" s="3"/>
@@ -2857,10 +2862,10 @@
       </c>
     </row>
     <row r="17" spans="1:26" ht="17" thickBot="1">
-      <c r="A17" s="18">
+      <c r="A17" s="17">
         <v>1</v>
       </c>
-      <c r="B17" s="18">
+      <c r="B17" s="17">
         <f t="shared" ref="B17" si="14">LEN(D17)-LEN(SUBSTITUTE(D17,",",""))+1</f>
         <v>1</v>
       </c>
@@ -2892,7 +2897,7 @@
       <c r="L17" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="M17" s="2" t="s">
+      <c r="M17" s="30" t="s">
         <v>38</v>
       </c>
       <c r="N17" s="2" t="s">
@@ -2943,8 +2948,8 @@
       </c>
     </row>
     <row r="18" spans="1:26" ht="17" thickBot="1">
-      <c r="A18" s="16"/>
-      <c r="B18" s="16"/>
+      <c r="A18" s="15"/>
+      <c r="B18" s="15"/>
       <c r="C18" s="4"/>
       <c r="D18" s="4"/>
       <c r="E18" s="3"/>
@@ -2955,7 +2960,7 @@
       <c r="J18" s="3"/>
       <c r="K18" s="3"/>
       <c r="L18" s="3"/>
-      <c r="M18" s="2"/>
+      <c r="M18" s="30"/>
       <c r="N18" s="2"/>
       <c r="O18" s="3"/>
       <c r="P18" s="3"/>
@@ -2992,10 +2997,10 @@
       </c>
     </row>
     <row r="19" spans="1:26" ht="29" thickBot="1">
-      <c r="A19" s="18">
+      <c r="A19" s="17">
         <v>1</v>
       </c>
-      <c r="B19" s="18">
+      <c r="B19" s="17">
         <f t="shared" ref="B19" si="16">LEN(D19)-LEN(SUBSTITUTE(D19,",",""))+1</f>
         <v>1</v>
       </c>
@@ -3023,7 +3028,7 @@
       <c r="L19" s="3" t="s">
         <v>108</v>
       </c>
-      <c r="M19" s="2" t="s">
+      <c r="M19" s="30" t="s">
         <v>104</v>
       </c>
       <c r="N19" s="2" t="s">
@@ -3076,10 +3081,10 @@
       </c>
     </row>
     <row r="20" spans="1:26" ht="17" thickBot="1">
-      <c r="A20" s="18">
+      <c r="A20" s="17">
         <v>5</v>
       </c>
-      <c r="B20" s="18">
+      <c r="B20" s="17">
         <v>5</v>
       </c>
       <c r="C20" s="4" t="s">
@@ -3104,7 +3109,7 @@
       <c r="L20" s="3" t="s">
         <v>198</v>
       </c>
-      <c r="M20" s="2" t="s">
+      <c r="M20" s="30" t="s">
         <v>89</v>
       </c>
       <c r="N20" s="3" t="s">
@@ -3155,10 +3160,10 @@
       </c>
     </row>
     <row r="21" spans="1:26" ht="29" thickBot="1">
-      <c r="A21" s="18">
+      <c r="A21" s="17">
         <v>4</v>
       </c>
-      <c r="B21" s="18">
+      <c r="B21" s="17">
         <v>4</v>
       </c>
       <c r="C21" s="4" t="s">
@@ -3187,7 +3192,7 @@
       <c r="L21" s="3" t="s">
         <v>258</v>
       </c>
-      <c r="M21" s="2" t="s">
+      <c r="M21" s="30" t="s">
         <v>100</v>
       </c>
       <c r="N21" s="2" t="s">
@@ -3196,7 +3201,7 @@
       <c r="O21" s="6">
         <v>0.56000000000000005</v>
       </c>
-      <c r="P21" s="25">
+      <c r="P21" s="24">
         <v>2.95</v>
       </c>
       <c r="Q21" s="6">
@@ -3239,11 +3244,11 @@
         <v>PREC040SAAN-RC.. 4</v>
       </c>
     </row>
-    <row r="22" spans="1:26" ht="43" thickBot="1">
-      <c r="A22" s="18">
+    <row r="22" spans="1:26" ht="57" thickBot="1">
+      <c r="A22" s="17">
         <v>1</v>
       </c>
-      <c r="B22" s="18">
+      <c r="B22" s="17">
         <v>1</v>
       </c>
       <c r="C22" s="4" t="s">
@@ -3272,7 +3277,7 @@
       <c r="L22" s="3" t="s">
         <v>174</v>
       </c>
-      <c r="M22" s="2" t="s">
+      <c r="M22" s="30" t="s">
         <v>170</v>
       </c>
       <c r="N22" s="2" t="s">
@@ -3323,8 +3328,8 @@
       </c>
     </row>
     <row r="23" spans="1:26" ht="17" thickBot="1">
-      <c r="A23" s="16"/>
-      <c r="B23" s="16"/>
+      <c r="A23" s="15"/>
+      <c r="B23" s="15"/>
       <c r="C23" s="4"/>
       <c r="D23" s="4"/>
       <c r="E23" s="3"/>
@@ -3335,7 +3340,7 @@
       <c r="J23" s="3"/>
       <c r="K23" s="3"/>
       <c r="L23" s="3"/>
-      <c r="M23" s="2"/>
+      <c r="M23" s="30"/>
       <c r="N23" s="2"/>
       <c r="O23" s="3"/>
       <c r="P23" s="3"/>
@@ -3366,18 +3371,18 @@
       </c>
     </row>
     <row r="24" spans="1:26" ht="29" thickBot="1">
-      <c r="A24" s="18">
+      <c r="A24" s="17">
         <f>LEN(C24)-LEN(SUBSTITUTE(C24,",",""))+1</f>
         <v>8</v>
       </c>
-      <c r="B24" s="18">
+      <c r="B24" s="17">
         <f t="shared" ref="B24" si="20">LEN(D24)-LEN(SUBSTITUTE(D24,",",""))+1</f>
         <v>6</v>
       </c>
       <c r="C24" s="4" t="s">
         <v>228</v>
       </c>
-      <c r="D24" s="22" t="s">
+      <c r="D24" s="21" t="s">
         <v>129</v>
       </c>
       <c r="E24" s="3" t="s">
@@ -3402,7 +3407,7 @@
       <c r="L24" s="3" t="s">
         <v>255</v>
       </c>
-      <c r="M24" s="2" t="s">
+      <c r="M24" s="30" t="s">
         <v>256</v>
       </c>
       <c r="N24" s="2" t="s">
@@ -3453,8 +3458,8 @@
       </c>
     </row>
     <row r="25" spans="1:26" ht="17" thickBot="1">
-      <c r="A25" s="16"/>
-      <c r="B25" s="16"/>
+      <c r="A25" s="15"/>
+      <c r="B25" s="15"/>
       <c r="C25" s="4"/>
       <c r="D25" s="4"/>
       <c r="E25" s="3"/>
@@ -3465,7 +3470,7 @@
       <c r="J25" s="3"/>
       <c r="K25" s="3"/>
       <c r="L25" s="3"/>
-      <c r="M25" s="2"/>
+      <c r="M25" s="30"/>
       <c r="N25" s="2"/>
       <c r="O25" s="3"/>
       <c r="P25" s="3"/>
@@ -3492,11 +3497,11 @@
       </c>
     </row>
     <row r="26" spans="1:26" ht="17" thickBot="1">
-      <c r="A26" s="18">
+      <c r="A26" s="17">
         <f>LEN(C26)-LEN(SUBSTITUTE(C26,",",""))+1</f>
         <v>1</v>
       </c>
-      <c r="B26" s="18">
+      <c r="B26" s="17">
         <f t="shared" ref="A26:B31" si="21">LEN(D26)-LEN(SUBSTITUTE(D26,",",""))+1</f>
         <v>1</v>
       </c>
@@ -3526,7 +3531,7 @@
       <c r="L26" s="3" t="s">
         <v>236</v>
       </c>
-      <c r="M26" s="2" t="s">
+      <c r="M26" s="30" t="s">
         <v>44</v>
       </c>
       <c r="N26" s="2" t="s">
@@ -3577,18 +3582,18 @@
       </c>
     </row>
     <row r="27" spans="1:26" ht="29" thickBot="1">
-      <c r="A27" s="18">
+      <c r="A27" s="17">
         <f>LEN(C27)-LEN(SUBSTITUTE(C27,",",""))+1</f>
         <v>17</v>
       </c>
-      <c r="B27" s="18">
+      <c r="B27" s="17">
         <f t="shared" si="21"/>
         <v>13</v>
       </c>
       <c r="C27" s="4" t="s">
         <v>246</v>
       </c>
-      <c r="D27" s="22" t="s">
+      <c r="D27" s="21" t="s">
         <v>247</v>
       </c>
       <c r="E27" s="3" t="s">
@@ -3611,7 +3616,7 @@
       <c r="L27" s="3" t="s">
         <v>235</v>
       </c>
-      <c r="M27" s="2" t="s">
+      <c r="M27" s="30" t="s">
         <v>47</v>
       </c>
       <c r="N27" s="2" t="s">
@@ -3662,48 +3667,48 @@
       </c>
     </row>
     <row r="28" spans="1:26" ht="17" thickBot="1">
-      <c r="A28" s="18">
+      <c r="A28" s="17">
         <f>LEN(C28)-LEN(SUBSTITUTE(C28,",",""))+1</f>
         <v>4</v>
       </c>
-      <c r="B28" s="18">
+      <c r="B28" s="17">
         <f t="shared" si="21"/>
         <v>2</v>
       </c>
-      <c r="C28" s="12" t="s">
+      <c r="C28" s="11" t="s">
         <v>248</v>
       </c>
-      <c r="D28" s="23" t="s">
+      <c r="D28" s="22" t="s">
         <v>250</v>
       </c>
-      <c r="E28" s="13">
+      <c r="E28" s="12">
         <v>680</v>
       </c>
       <c r="F28" s="7" t="s">
         <v>137</v>
       </c>
       <c r="G28" s="3"/>
-      <c r="H28" s="13"/>
-      <c r="I28" s="13"/>
-      <c r="J28" s="13" t="s">
+      <c r="H28" s="12"/>
+      <c r="I28" s="12"/>
+      <c r="J28" s="12" t="s">
         <v>138</v>
       </c>
-      <c r="K28" s="13" t="s">
+      <c r="K28" s="12" t="s">
         <v>158</v>
       </c>
-      <c r="L28" s="7" t="s">
+      <c r="L28" s="12" t="s">
         <v>233</v>
       </c>
-      <c r="M28" s="2" t="s">
+      <c r="M28" s="30" t="s">
         <v>136</v>
       </c>
       <c r="N28" s="2" t="s">
         <v>202</v>
       </c>
-      <c r="O28" s="14">
+      <c r="O28" s="13">
         <v>0.22</v>
       </c>
-      <c r="P28" s="14">
+      <c r="P28" s="13">
         <v>0.15</v>
       </c>
       <c r="Q28" s="6">
@@ -3722,7 +3727,7 @@
         <f t="shared" si="5"/>
         <v>0.3</v>
       </c>
-      <c r="U28" s="12" t="s">
+      <c r="U28" s="11" t="s">
         <v>99</v>
       </c>
       <c r="V28" s="4" t="str">
@@ -3747,11 +3752,11 @@
       </c>
     </row>
     <row r="29" spans="1:26" ht="29" thickBot="1">
-      <c r="A29" s="18">
+      <c r="A29" s="17">
         <f>LEN(C29)-LEN(SUBSTITUTE(C29,",",""))+1</f>
         <v>6</v>
       </c>
-      <c r="B29" s="18">
+      <c r="B29" s="17">
         <f t="shared" si="21"/>
         <v>6</v>
       </c>
@@ -3778,10 +3783,10 @@
       <c r="K29" s="3" t="s">
         <v>158</v>
       </c>
-      <c r="L29" s="7" t="s">
+      <c r="L29" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="M29" s="2" t="s">
+      <c r="M29" s="30" t="s">
         <v>51</v>
       </c>
       <c r="N29" s="2" t="s">
@@ -3790,7 +3795,7 @@
       <c r="O29" s="5">
         <v>0.11</v>
       </c>
-      <c r="P29" s="14">
+      <c r="P29" s="13">
         <v>0.15</v>
       </c>
       <c r="Q29" s="6">
@@ -3832,11 +3837,11 @@
       </c>
     </row>
     <row r="30" spans="1:26" ht="29" thickBot="1">
-      <c r="A30" s="18">
+      <c r="A30" s="17">
         <f t="shared" si="21"/>
         <v>7</v>
       </c>
-      <c r="B30" s="18">
+      <c r="B30" s="17">
         <f t="shared" si="21"/>
         <v>5</v>
       </c>
@@ -3868,7 +3873,7 @@
       <c r="L30" s="3" t="s">
         <v>240</v>
       </c>
-      <c r="M30" s="2" t="s">
+      <c r="M30" s="30" t="s">
         <v>237</v>
       </c>
       <c r="N30" s="2" t="s">
@@ -3919,10 +3924,10 @@
       </c>
     </row>
     <row r="31" spans="1:26" ht="17" thickBot="1">
-      <c r="A31" s="18">
+      <c r="A31" s="17">
         <v>1</v>
       </c>
-      <c r="B31" s="18">
+      <c r="B31" s="17">
         <f t="shared" si="21"/>
         <v>1</v>
       </c>
@@ -3952,7 +3957,7 @@
       <c r="L31" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="M31" s="2" t="s">
+      <c r="M31" s="30" t="s">
         <v>55</v>
       </c>
       <c r="N31" s="2" t="s">
@@ -4005,18 +4010,18 @@
       </c>
     </row>
     <row r="32" spans="1:26" ht="17" thickBot="1">
-      <c r="A32" s="18">
+      <c r="A32" s="17">
         <f t="shared" ref="A32:A33" si="25">LEN(C32)-LEN(SUBSTITUTE(C32,",",""))+1</f>
         <v>12</v>
       </c>
-      <c r="B32" s="18">
+      <c r="B32" s="17">
         <f>LEN(D32)-LEN(SUBSTITUTE(D32,",",""))+1</f>
         <v>8</v>
       </c>
       <c r="C32" s="4" t="s">
         <v>230</v>
       </c>
-      <c r="D32" s="22" t="s">
+      <c r="D32" s="21" t="s">
         <v>134</v>
       </c>
       <c r="E32" s="3" t="s">
@@ -4039,7 +4044,7 @@
       <c r="L32" s="3" t="s">
         <v>260</v>
       </c>
-      <c r="M32" s="2" t="s">
+      <c r="M32" s="30" t="s">
         <v>58</v>
       </c>
       <c r="N32" s="2" t="s">
@@ -4089,19 +4094,19 @@
         <v>MFR-25FBF52-100K 12</v>
       </c>
     </row>
-    <row r="33" spans="1:26" ht="17" thickBot="1">
-      <c r="A33" s="18">
+    <row r="33" spans="1:26" ht="29" thickBot="1">
+      <c r="A33" s="17">
         <f t="shared" si="25"/>
         <v>4</v>
       </c>
-      <c r="B33" s="18">
+      <c r="B33" s="17">
         <f>LEN(D33)-LEN(SUBSTITUTE(D33,",",""))+1</f>
         <v>2</v>
       </c>
       <c r="C33" s="4" t="s">
         <v>231</v>
       </c>
-      <c r="D33" s="22" t="s">
+      <c r="D33" s="21" t="s">
         <v>132</v>
       </c>
       <c r="E33" s="3">
@@ -4124,7 +4129,7 @@
       <c r="L33" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="M33" s="2" t="s">
+      <c r="M33" s="30" t="s">
         <v>61</v>
       </c>
       <c r="N33" s="2" t="s">
@@ -4175,8 +4180,8 @@
       </c>
     </row>
     <row r="34" spans="1:26" ht="17" thickBot="1">
-      <c r="A34" s="16"/>
-      <c r="B34" s="16"/>
+      <c r="A34" s="15"/>
+      <c r="B34" s="15"/>
       <c r="C34" s="4"/>
       <c r="D34" s="4"/>
       <c r="E34" s="3"/>
@@ -4187,7 +4192,7 @@
       <c r="J34" s="3"/>
       <c r="K34" s="3"/>
       <c r="L34" s="3"/>
-      <c r="M34" s="2"/>
+      <c r="M34" s="30"/>
       <c r="N34" s="2"/>
       <c r="O34" s="3"/>
       <c r="P34" s="3"/>
@@ -4214,10 +4219,10 @@
       </c>
     </row>
     <row r="35" spans="1:26" ht="29" thickBot="1">
-      <c r="A35" s="18">
+      <c r="A35" s="17">
         <v>1</v>
       </c>
-      <c r="B35" s="18">
+      <c r="B35" s="17">
         <f t="shared" ref="B35:B37" si="26">LEN(D35)-LEN(SUBSTITUTE(D35,",",""))+1</f>
         <v>1</v>
       </c>
@@ -4249,7 +4254,7 @@
       <c r="L35" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="M35" s="2" t="s">
+      <c r="M35" s="30" t="s">
         <v>64</v>
       </c>
       <c r="N35" s="2" t="s">
@@ -4300,10 +4305,10 @@
       </c>
     </row>
     <row r="36" spans="1:26" ht="29" thickBot="1">
-      <c r="A36" s="18">
+      <c r="A36" s="17">
         <v>1</v>
       </c>
-      <c r="B36" s="18">
+      <c r="B36" s="17">
         <f t="shared" si="26"/>
         <v>1</v>
       </c>
@@ -4333,7 +4338,7 @@
       <c r="L36" s="3" t="s">
         <v>182</v>
       </c>
-      <c r="M36" s="2" t="s">
+      <c r="M36" s="30" t="s">
         <v>80</v>
       </c>
       <c r="N36" s="2" t="s">
@@ -4384,51 +4389,51 @@
       </c>
     </row>
     <row r="37" spans="1:26" ht="29" thickBot="1">
-      <c r="A37" s="18">
+      <c r="A37" s="17">
         <v>2</v>
       </c>
-      <c r="B37" s="18">
+      <c r="B37" s="17">
         <f t="shared" si="26"/>
         <v>1</v>
       </c>
-      <c r="C37" s="12" t="s">
+      <c r="C37" s="11" t="s">
         <v>232</v>
       </c>
-      <c r="D37" s="12" t="s">
+      <c r="D37" s="11" t="s">
         <v>133</v>
       </c>
-      <c r="E37" s="13" t="s">
+      <c r="E37" s="12" t="s">
         <v>124</v>
       </c>
-      <c r="F37" s="13" t="s">
+      <c r="F37" s="12" t="s">
         <v>125</v>
       </c>
       <c r="G37" s="3" t="s">
         <v>126</v>
       </c>
-      <c r="H37" s="13"/>
-      <c r="I37" s="13">
+      <c r="H37" s="12"/>
+      <c r="I37" s="12">
         <v>2</v>
       </c>
-      <c r="J37" s="13" t="s">
+      <c r="J37" s="12" t="s">
         <v>68</v>
       </c>
-      <c r="K37" s="13" t="s">
+      <c r="K37" s="12" t="s">
         <v>158</v>
       </c>
-      <c r="L37" s="13" t="s">
+      <c r="L37" s="12" t="s">
         <v>124</v>
       </c>
-      <c r="M37" s="13" t="s">
+      <c r="M37" s="12" t="s">
         <v>127</v>
       </c>
-      <c r="N37" s="13" t="s">
+      <c r="N37" s="12" t="s">
         <v>184</v>
       </c>
-      <c r="O37" s="20">
+      <c r="O37" s="19">
         <v>2.92</v>
       </c>
-      <c r="P37" s="20">
+      <c r="P37" s="19">
         <v>2.92</v>
       </c>
       <c r="Q37" s="6">
@@ -4447,7 +4452,7 @@
         <f t="shared" si="5"/>
         <v>2.92</v>
       </c>
-      <c r="U37" s="12"/>
+      <c r="U37" s="11"/>
       <c r="V37" s="4" t="str">
         <f t="shared" si="19"/>
         <v>2,TC4424EPA-ND</v>
@@ -4470,19 +4475,19 @@
       </c>
     </row>
     <row r="38" spans="1:26" ht="17" thickBot="1">
-      <c r="A38" s="18">
+      <c r="A38" s="17">
         <v>1</v>
       </c>
-      <c r="B38" s="27">
+      <c r="B38" s="26">
         <v>1</v>
       </c>
-      <c r="C38" s="12" t="s">
+      <c r="C38" s="11" t="s">
         <v>167</v>
       </c>
-      <c r="D38" s="12" t="s">
+      <c r="D38" s="11" t="s">
         <v>167</v>
       </c>
-      <c r="E38" s="13" t="s">
+      <c r="E38" s="12" t="s">
         <v>216</v>
       </c>
       <c r="F38" s="3" t="s">
@@ -4491,20 +4496,20 @@
       <c r="G38" s="3" t="s">
         <v>126</v>
       </c>
-      <c r="H38" s="13"/>
-      <c r="I38" s="13">
+      <c r="H38" s="12"/>
+      <c r="I38" s="12">
         <v>1</v>
       </c>
-      <c r="J38" s="13" t="s">
+      <c r="J38" s="12" t="s">
         <v>218</v>
       </c>
-      <c r="K38" s="26" t="s">
+      <c r="K38" s="25" t="s">
         <v>158</v>
       </c>
-      <c r="L38" s="13" t="s">
+      <c r="L38" s="12" t="s">
         <v>216</v>
       </c>
-      <c r="M38" s="13" t="s">
+      <c r="M38" s="12" t="s">
         <v>219</v>
       </c>
       <c r="N38" s="2" t="s">
@@ -4555,33 +4560,33 @@
       </c>
     </row>
     <row r="39" spans="1:26" ht="17" thickBot="1">
-      <c r="A39" s="18">
+      <c r="A39" s="17">
         <v>3</v>
       </c>
-      <c r="B39" s="27">
+      <c r="B39" s="26">
         <v>2</v>
       </c>
-      <c r="C39" s="12" t="s">
+      <c r="C39" s="11" t="s">
         <v>86</v>
       </c>
-      <c r="D39" s="12" t="s">
+      <c r="D39" s="11" t="s">
         <v>86</v>
       </c>
-      <c r="E39" s="13" t="s">
+      <c r="E39" s="12" t="s">
         <v>119</v>
       </c>
       <c r="F39" s="3"/>
       <c r="G39" s="3"/>
-      <c r="H39" s="13"/>
-      <c r="I39" s="13"/>
-      <c r="J39" s="13"/>
-      <c r="K39" s="26" t="s">
+      <c r="H39" s="12"/>
+      <c r="I39" s="12"/>
+      <c r="J39" s="12"/>
+      <c r="K39" s="25" t="s">
         <v>158</v>
       </c>
-      <c r="L39" s="13" t="s">
+      <c r="L39" s="12" t="s">
         <v>85</v>
       </c>
-      <c r="M39" s="13" t="s">
+      <c r="M39" s="12" t="s">
         <v>84</v>
       </c>
       <c r="N39" s="2" t="s">
@@ -4632,8 +4637,8 @@
       </c>
     </row>
     <row r="40" spans="1:26" ht="17" thickBot="1">
-      <c r="A40" s="16"/>
-      <c r="B40" s="16"/>
+      <c r="A40" s="15"/>
+      <c r="B40" s="15"/>
       <c r="C40" s="4"/>
       <c r="D40" s="4"/>
       <c r="E40" s="3"/>
@@ -4643,16 +4648,16 @@
       <c r="I40" s="4"/>
       <c r="J40" s="4"/>
       <c r="K40" s="4"/>
-      <c r="L40" s="9"/>
-      <c r="M40" s="3"/>
+      <c r="L40" s="4"/>
+      <c r="M40" s="12"/>
       <c r="N40" s="3"/>
       <c r="O40" s="1"/>
       <c r="P40" s="1"/>
-      <c r="Q40" s="10"/>
+      <c r="Q40" s="9"/>
       <c r="R40" s="6"/>
-      <c r="S40" s="10"/>
+      <c r="S40" s="9"/>
       <c r="T40" s="6"/>
-      <c r="U40" s="10"/>
+      <c r="U40" s="9"/>
       <c r="V40" s="4" t="str">
         <f t="shared" si="33"/>
         <v/>
@@ -4667,10 +4672,10 @@
       </c>
     </row>
     <row r="41" spans="1:26" ht="29" thickBot="1">
-      <c r="A41" s="16">
+      <c r="A41" s="15">
         <v>1</v>
       </c>
-      <c r="B41" s="16">
+      <c r="B41" s="15">
         <v>1</v>
       </c>
       <c r="C41" s="4" t="s">
@@ -4693,10 +4698,10 @@
       <c r="L41" s="3" t="s">
         <v>165</v>
       </c>
-      <c r="M41" s="13" t="s">
+      <c r="M41" s="12" t="s">
         <v>164</v>
       </c>
-      <c r="N41" s="13" t="s">
+      <c r="N41" s="12" t="s">
         <v>209</v>
       </c>
       <c r="O41" s="6">
@@ -4721,7 +4726,7 @@
         <f t="shared" si="5"/>
         <v>15.33</v>
       </c>
-      <c r="U41" s="10"/>
+      <c r="U41" s="9"/>
       <c r="V41" s="4" t="str">
         <f t="shared" si="33"/>
         <v>1,HM975-ND</v>
@@ -4736,8 +4741,8 @@
       </c>
     </row>
     <row r="42" spans="1:26" ht="17" thickBot="1">
-      <c r="A42" s="16"/>
-      <c r="B42" s="16"/>
+      <c r="A42" s="15"/>
+      <c r="B42" s="15"/>
       <c r="C42" s="4"/>
       <c r="D42" s="4"/>
       <c r="E42" s="3"/>
@@ -4747,16 +4752,16 @@
       <c r="I42" s="4"/>
       <c r="J42" s="4"/>
       <c r="K42" s="4"/>
-      <c r="L42" s="9"/>
-      <c r="M42" s="3"/>
+      <c r="L42" s="4"/>
+      <c r="M42" s="12"/>
       <c r="N42" s="3"/>
       <c r="O42" s="1"/>
       <c r="P42" s="1"/>
-      <c r="Q42" s="10"/>
+      <c r="Q42" s="9"/>
       <c r="R42" s="6"/>
-      <c r="S42" s="10"/>
-      <c r="T42" s="10"/>
-      <c r="U42" s="10"/>
+      <c r="S42" s="9"/>
+      <c r="T42" s="9"/>
+      <c r="U42" s="9"/>
       <c r="V42" s="4" t="str">
         <f t="shared" si="33"/>
         <v/>
@@ -4767,8 +4772,8 @@
       </c>
     </row>
     <row r="43" spans="1:26" ht="17" thickBot="1">
-      <c r="A43" s="16"/>
-      <c r="B43" s="16"/>
+      <c r="A43" s="15"/>
+      <c r="B43" s="15"/>
       <c r="C43" s="4" t="s">
         <v>71</v>
       </c>
@@ -4778,12 +4783,12 @@
       <c r="E43" s="3"/>
       <c r="F43" s="3"/>
       <c r="G43" s="3"/>
-      <c r="H43" s="21"/>
+      <c r="H43" s="20"/>
       <c r="I43" s="8"/>
       <c r="J43" s="4"/>
       <c r="K43" s="8"/>
       <c r="L43" s="4"/>
-      <c r="M43" s="3"/>
+      <c r="M43" s="12"/>
       <c r="N43" s="3"/>
       <c r="O43" s="4"/>
       <c r="P43" s="4"/>
@@ -4802,10 +4807,10 @@
       </c>
     </row>
     <row r="44" spans="1:26" ht="17" thickBot="1">
-      <c r="A44" s="16">
+      <c r="A44" s="15">
         <v>1</v>
       </c>
-      <c r="B44" s="16"/>
+      <c r="B44" s="15"/>
       <c r="C44" s="4" t="s">
         <v>169</v>
       </c>
@@ -4828,7 +4833,7 @@
       <c r="L44" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="M44" s="3"/>
+      <c r="M44" s="12"/>
       <c r="N44" s="3"/>
       <c r="O44" s="6">
         <v>15</v>
@@ -4853,11 +4858,11 @@
       </c>
       <c r="W44" s="4"/>
     </row>
-    <row r="45" spans="1:26" ht="17" thickBot="1">
-      <c r="A45" s="16">
+    <row r="45" spans="1:26" ht="29" thickBot="1">
+      <c r="A45" s="15">
         <v>1</v>
       </c>
-      <c r="B45" s="16"/>
+      <c r="B45" s="15"/>
       <c r="C45" s="4" t="s">
         <v>92</v>
       </c>
@@ -4872,7 +4877,7 @@
       <c r="J45" s="3"/>
       <c r="K45" s="3"/>
       <c r="L45" s="3"/>
-      <c r="M45" s="3" t="s">
+      <c r="M45" s="12" t="s">
         <v>91</v>
       </c>
       <c r="N45" s="3"/>
@@ -4889,43 +4894,43 @@
       </c>
     </row>
     <row r="46" spans="1:26" ht="17" thickBot="1">
-      <c r="A46" s="16"/>
-      <c r="B46" s="16"/>
+      <c r="A46" s="15"/>
+      <c r="B46" s="15"/>
       <c r="C46" s="4"/>
       <c r="D46" s="4"/>
       <c r="E46" s="3"/>
       <c r="F46" s="3"/>
       <c r="G46" s="3"/>
-      <c r="H46" s="21"/>
+      <c r="H46" s="20"/>
       <c r="I46" s="8"/>
       <c r="J46" s="4"/>
       <c r="K46" s="8"/>
-      <c r="L46" s="28" t="s">
+      <c r="L46" s="27" t="s">
         <v>74</v>
       </c>
-      <c r="M46" s="29"/>
-      <c r="N46" s="24"/>
+      <c r="M46" s="28"/>
+      <c r="N46" s="23"/>
       <c r="O46" s="1" t="s">
         <v>69</v>
       </c>
       <c r="P46" s="1"/>
-      <c r="Q46" s="11">
+      <c r="Q46" s="10">
         <f>SUM(Q2:Q45)</f>
         <v>98.992000000000004</v>
       </c>
-      <c r="R46" s="11">
+      <c r="R46" s="10">
         <f>SUM(R2:R45)</f>
         <v>106.4</v>
       </c>
-      <c r="S46" s="11">
+      <c r="S46" s="10">
         <f>SUM(S2:S45)</f>
         <v>72.89200000000001</v>
       </c>
-      <c r="T46" s="11">
+      <c r="T46" s="10">
         <f>SUM(T2:T45)</f>
         <v>82.16</v>
       </c>
-      <c r="U46" s="10" t="s">
+      <c r="U46" s="9" t="s">
         <v>70</v>
       </c>
     </row>
@@ -4948,7 +4953,7 @@
     <hyperlink ref="M32" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
   </hyperlinks>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" scale="62" orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <pageSetup paperSize="9" scale="27" orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <legacyDrawing r:id="rId12"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Minor parts updates for v0.4 BOM
</commit_message>
<xml_diff>
--- a/reference/hardware/v0.4/BOMs/v0.4.3_bom.xlsx
+++ b/reference/hardware/v0.4/BOMs/v0.4.3_bom.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10614"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11110"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/josh/Documents/Arduino/speeduino/reference/hardware/v0.4/BOMs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9F7BE8A-8FA2-6342-8CEB-CFB1EE678473}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E049360-306A-2946-8153-FD5D49F4FB9C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="600" yWindow="520" windowWidth="28800" windowHeight="16060" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16000" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Component List" sheetId="1" r:id="rId1"/>
@@ -94,7 +94,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="338" uniqueCount="264">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="337" uniqueCount="263">
   <si>
     <t>Value</t>
   </si>
@@ -261,15 +261,6 @@
     <t>100KXBK-ND</t>
   </si>
   <si>
-    <t>RES 160 OHM 2W 1% AXIAL</t>
-  </si>
-  <si>
-    <t>FMP200FRF52-160R</t>
-  </si>
-  <si>
-    <t>160YCT-ND</t>
-  </si>
-  <si>
     <t>U1</t>
   </si>
   <si>
@@ -696,9 +687,6 @@
     <t>279-H83K9BDA</t>
   </si>
   <si>
-    <t>594-5083NW160R0J</t>
-  </si>
-  <si>
     <t>CTM Full Digikey</t>
   </si>
   <si>
@@ -876,16 +864,25 @@
     <t>BC3323-ND</t>
   </si>
   <si>
-    <t>MOV-20D220K</t>
-  </si>
-  <si>
-    <t>MOV-20D220K-ND</t>
-  </si>
-  <si>
     <t>Bournes Inc</t>
   </si>
   <si>
-    <t>SURGE ABSORBER 20MM 22V 1000A ZNR</t>
+    <t>F6389-ND</t>
+  </si>
+  <si>
+    <t>V14E14AUTO</t>
+  </si>
+  <si>
+    <t>VARISTOR 22V 3KA DISC 14MM</t>
+  </si>
+  <si>
+    <t>FMP200JR-52-10R</t>
+  </si>
+  <si>
+    <t>10ZCT-ND</t>
+  </si>
+  <si>
+    <t>RES 10 OHM 2W 5% AXIAL</t>
   </si>
 </sst>
 </file>
@@ -1603,8 +1600,8 @@
   </sheetPr>
   <dimension ref="A1:Z46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="57" workbookViewId="0">
-      <selection activeCell="G26" sqref="G26"/>
+    <sheetView tabSelected="1" topLeftCell="A14" zoomScale="75" workbookViewId="0">
+      <selection activeCell="F32" sqref="F32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1628,16 +1625,16 @@
   <sheetData>
     <row r="1" spans="1:26" ht="29" thickBot="1">
       <c r="A1" s="14" t="s">
+        <v>153</v>
+      </c>
+      <c r="B1" s="14" t="s">
+        <v>154</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>156</v>
-      </c>
-      <c r="B1" s="14" t="s">
-        <v>157</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>158</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>159</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>0</v>
@@ -1649,7 +1646,7 @@
         <v>2</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>3</v>
@@ -1658,7 +1655,7 @@
         <v>4</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="L1" s="1" t="s">
         <v>5</v>
@@ -1667,40 +1664,40 @@
         <v>6</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="S1" s="1" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="T1" s="1" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="U1" s="1" t="s">
         <v>7</v>
       </c>
       <c r="V1" s="18" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="W1" s="18" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="X1" s="18" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="Y1" s="18" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
     </row>
     <row r="2" spans="1:26" ht="17" thickBot="1">
@@ -1748,16 +1745,16 @@
         <v>1</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="E3" s="3" t="s">
         <v>8</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="G3" s="3" t="s">
         <v>9</v>
@@ -1770,16 +1767,16 @@
         <v>13</v>
       </c>
       <c r="K3" s="3" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="L3" s="3" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="M3" s="28" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="N3" s="2" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="O3" s="5">
         <v>1.7</v>
@@ -1835,16 +1832,16 @@
         <v>6</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
       <c r="E4" s="3" t="s">
         <v>11</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="G4" s="3" t="s">
         <v>12</v>
@@ -1857,16 +1854,16 @@
         <v>13</v>
       </c>
       <c r="K4" s="3" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="L4" s="3" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="M4" s="28" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
       <c r="N4" s="2" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
       <c r="O4" s="5">
         <v>0.66</v>
@@ -1922,16 +1919,16 @@
         <v>7</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="E5" s="3" t="s">
         <v>14</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="G5" s="3" t="s">
         <v>12</v>
@@ -1941,19 +1938,19 @@
         <v>17</v>
       </c>
       <c r="J5" s="3" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
       <c r="K5" s="3" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="L5" s="3" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
       <c r="M5" s="28" t="s">
-        <v>259</v>
+        <v>255</v>
       </c>
       <c r="N5" s="2" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="O5" s="5">
         <v>0.36</v>
@@ -2009,16 +2006,16 @@
         <v>1</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="E6" s="3" t="s">
         <v>15</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="G6" s="3" t="s">
         <v>9</v>
@@ -2031,16 +2028,16 @@
         <v>13</v>
       </c>
       <c r="K6" s="3" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="L6" s="3" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="M6" s="28" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="N6" s="2" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="O6" s="5">
         <v>1.57</v>
@@ -2096,16 +2093,16 @@
         <v>1</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="E7" s="3" t="s">
         <v>16</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="G7" s="3" t="s">
         <v>12</v>
@@ -2118,16 +2115,16 @@
         <v>10</v>
       </c>
       <c r="K7" s="3" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="L7" s="3" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="M7" s="28" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="N7" s="2" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="O7" s="5">
         <v>0.62</v>
@@ -2183,16 +2180,16 @@
         <v>2</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
       <c r="E8" s="3" t="s">
         <v>17</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="G8" s="3" t="s">
         <v>12</v>
@@ -2205,16 +2202,16 @@
         <v>13</v>
       </c>
       <c r="K8" s="3" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="L8" s="3" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="M8" s="28" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="N8" s="2" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="O8" s="5">
         <v>0.24</v>
@@ -2270,16 +2267,16 @@
         <v>2</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="D9" s="21" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="E9" s="3" t="s">
         <v>18</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="G9" s="3" t="s">
         <v>12</v>
@@ -2292,16 +2289,16 @@
         <v>13</v>
       </c>
       <c r="K9" s="3" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="L9" s="3" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="M9" s="28" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="N9" s="2" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="O9" s="5">
         <v>0.66</v>
@@ -2357,16 +2354,16 @@
         <v>1</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="E10" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="F10" s="3" t="s">
         <v>107</v>
-      </c>
-      <c r="F10" s="3" t="s">
-        <v>110</v>
       </c>
       <c r="G10" s="3" t="s">
         <v>12</v>
@@ -2377,16 +2374,16 @@
         <v>13</v>
       </c>
       <c r="K10" s="3" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="L10" s="3" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="M10" s="28" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="N10" s="2" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="O10" s="5">
         <v>0.25</v>
@@ -2481,13 +2478,13 @@
         <v>1</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="F12" s="7" t="s">
         <v>19</v>
@@ -2503,7 +2500,7 @@
         <v>21</v>
       </c>
       <c r="K12" s="3" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="L12" s="3" t="s">
         <v>22</v>
@@ -2512,7 +2509,7 @@
         <v>23</v>
       </c>
       <c r="N12" s="2" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="O12" s="5">
         <v>0.34</v>
@@ -2568,13 +2565,13 @@
         <v>2</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="F13" s="3" t="s">
         <v>25</v>
@@ -2590,7 +2587,7 @@
         <v>26</v>
       </c>
       <c r="K13" s="3" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="L13" s="3" t="s">
         <v>24</v>
@@ -2599,7 +2596,7 @@
         <v>27</v>
       </c>
       <c r="N13" s="2" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="O13" s="5">
         <v>0.39</v>
@@ -2655,34 +2652,34 @@
         <v>4</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="D14" s="21" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="E14" s="3" t="s">
         <v>28</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="G14" s="3" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="H14" s="3"/>
       <c r="I14" s="3"/>
       <c r="J14" s="3"/>
       <c r="K14" s="3" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="L14" s="3" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
       <c r="M14" s="28" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="N14" s="2" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="O14" s="5">
         <v>0.47</v>
@@ -2738,10 +2735,10 @@
         <v>2</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
       <c r="D15" s="21" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="E15" s="3" t="s">
         <v>29</v>
@@ -2760,7 +2757,7 @@
         <v>26</v>
       </c>
       <c r="K15" s="3" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="L15" s="3" t="s">
         <v>31</v>
@@ -2769,7 +2766,7 @@
         <v>32</v>
       </c>
       <c r="N15" s="2" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="O15" s="5">
         <v>0.11</v>
@@ -2867,16 +2864,16 @@
         <v>1</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="E17" s="3" t="s">
         <v>33</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
       <c r="G17" s="3" t="s">
         <v>34</v>
@@ -2886,16 +2883,16 @@
         <v>1</v>
       </c>
       <c r="J17" s="3" t="s">
-        <v>262</v>
+        <v>256</v>
       </c>
       <c r="K17" s="3" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="L17" s="3" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="M17" s="28" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
       <c r="N17" s="2"/>
       <c r="O17" s="5">
@@ -2923,11 +2920,11 @@
       <c r="U17" s="4"/>
       <c r="V17" s="4" t="str">
         <f>IF(NOT(M17=""),A17&amp;","&amp;M17,"")</f>
-        <v>1,MOV-20D220K-ND</v>
+        <v>1,F6389-ND</v>
       </c>
       <c r="W17" s="4" t="str">
         <f>IF(NOT(M17=""),B17&amp;","&amp;M17,"")</f>
-        <v>1,MOV-20D220K-ND</v>
+        <v>1,F6389-ND</v>
       </c>
       <c r="X17" t="str">
         <f t="shared" si="13"/>
@@ -2939,7 +2936,7 @@
       </c>
       <c r="Z17" t="str">
         <f>L17&amp;" "&amp;A17</f>
-        <v>MOV-20D220K 1</v>
+        <v>V14E14AUTO 1</v>
       </c>
     </row>
     <row r="18" spans="1:26" ht="17" thickBot="1">
@@ -3000,34 +2997,34 @@
         <v>1</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="F19" s="3" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="G19" s="3"/>
       <c r="H19" s="3"/>
       <c r="I19" s="3"/>
       <c r="J19" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="K19" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="L19" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="K19" s="3" t="s">
-        <v>155</v>
-      </c>
-      <c r="L19" s="3" t="s">
-        <v>104</v>
-      </c>
       <c r="M19" s="28" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="N19" s="2" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="O19" s="3">
         <v>0.40200000000000002</v>
@@ -3052,7 +3049,7 @@
         <v>0.51</v>
       </c>
       <c r="U19" s="4" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="V19" s="4" t="str">
         <f t="shared" si="0"/>
@@ -3083,32 +3080,32 @@
         <v>5</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="E20" s="3" t="s">
         <v>35</v>
       </c>
       <c r="F20" s="3" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="G20" s="3"/>
       <c r="H20" s="3"/>
       <c r="I20" s="3"/>
       <c r="J20" s="3"/>
       <c r="K20" s="3" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="L20" s="3" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="M20" s="28" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="N20" s="3" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="O20" s="5">
         <v>0.1</v>
@@ -3162,16 +3159,16 @@
         <v>4</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="D21" s="4" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="F21" s="3" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="G21" s="3"/>
       <c r="H21" s="3"/>
@@ -3179,19 +3176,19 @@
         <v>1</v>
       </c>
       <c r="J21" s="3" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="K21" s="3" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="L21" s="3" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
       <c r="M21" s="28" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="N21" s="2" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
       <c r="O21" s="6">
         <v>0.56000000000000005</v>
@@ -3216,7 +3213,7 @@
         <v>11.8</v>
       </c>
       <c r="U21" s="4" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="V21" s="4" t="str">
         <f t="shared" si="0"/>
@@ -3247,16 +3244,16 @@
         <v>1</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="F22" s="3" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="G22" s="3"/>
       <c r="H22" s="3"/>
@@ -3264,19 +3261,19 @@
         <v>1</v>
       </c>
       <c r="J22" s="3" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="K22" s="3" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="L22" s="3" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="M22" s="28" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="N22" s="2" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="O22" s="6">
         <v>1.1299999999999999</v>
@@ -3375,19 +3372,19 @@
         <v>6</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="D24" s="21" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="F24" s="3" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
       <c r="G24" s="3" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="H24" s="3"/>
       <c r="I24" s="3">
@@ -3397,16 +3394,16 @@
         <v>36</v>
       </c>
       <c r="K24" s="3" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="L24" s="3" t="s">
-        <v>250</v>
+        <v>246</v>
       </c>
       <c r="M24" s="28" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="N24" s="2" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="O24" s="6">
         <v>1.51</v>
@@ -3501,10 +3498,10 @@
         <v>1</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
       <c r="D26" s="4" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
       <c r="E26" s="3" t="s">
         <v>37</v>
@@ -3521,16 +3518,16 @@
         <v>39</v>
       </c>
       <c r="K26" s="3" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="L26" s="3" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="M26" s="28" t="s">
         <v>40</v>
       </c>
       <c r="N26" s="2" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="O26" s="5">
         <v>0.08</v>
@@ -3586,10 +3583,10 @@
         <v>13</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="D27" s="21" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="E27" s="3" t="s">
         <v>41</v>
@@ -3606,16 +3603,16 @@
         <v>39</v>
       </c>
       <c r="K27" s="3" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="L27" s="3" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="M27" s="28" t="s">
         <v>43</v>
       </c>
       <c r="N27" s="2" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="O27" s="5">
         <v>0.06</v>
@@ -3671,34 +3668,34 @@
         <v>2</v>
       </c>
       <c r="C28" s="11" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
       <c r="D28" s="22" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
       <c r="E28" s="12">
         <v>680</v>
       </c>
       <c r="F28" s="7" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="G28" s="3"/>
       <c r="H28" s="12"/>
       <c r="I28" s="12"/>
       <c r="J28" s="12" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="K28" s="12" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="L28" s="12" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
       <c r="M28" s="28" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="N28" s="2" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="O28" s="13">
         <v>0.22</v>
@@ -3723,7 +3720,7 @@
         <v>0.3</v>
       </c>
       <c r="U28" s="11" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="V28" s="4" t="str">
         <f t="shared" si="19"/>
@@ -3756,10 +3753,10 @@
         <v>6</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="D29" s="4" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="E29" s="3">
         <v>470</v>
@@ -3776,7 +3773,7 @@
         <v>45</v>
       </c>
       <c r="K29" s="3" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="L29" s="3" t="s">
         <v>46</v>
@@ -3785,7 +3782,7 @@
         <v>47</v>
       </c>
       <c r="N29" s="2" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="O29" s="5">
         <v>0.11</v>
@@ -3841,16 +3838,16 @@
         <v>5</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>244</v>
+        <v>240</v>
       </c>
       <c r="D30" s="4" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
       <c r="E30" s="3" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
       <c r="F30" s="3" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="G30" s="3" t="s">
         <v>48</v>
@@ -3863,16 +3860,16 @@
         <v>39</v>
       </c>
       <c r="K30" s="3" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="L30" s="3" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="M30" s="28" t="s">
+        <v>228</v>
+      </c>
+      <c r="N30" s="2" t="s">
         <v>232</v>
-      </c>
-      <c r="N30" s="2" t="s">
-        <v>236</v>
       </c>
       <c r="O30" s="5">
         <v>0.14000000000000001</v>
@@ -3927,13 +3924,13 @@
         <v>1</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="D31" s="4" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="E31" s="3" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="F31" s="3" t="s">
         <v>49</v>
@@ -3947,7 +3944,7 @@
         <v>39</v>
       </c>
       <c r="K31" s="3" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="L31" s="3" t="s">
         <v>50</v>
@@ -3956,7 +3953,7 @@
         <v>51</v>
       </c>
       <c r="N31" s="2" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="O31" s="5">
         <v>0.46</v>
@@ -3981,7 +3978,7 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="U31" s="4" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="V31" s="4" t="str">
         <f t="shared" si="19"/>
@@ -4014,10 +4011,10 @@
         <v>8</v>
       </c>
       <c r="C32" s="4" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
       <c r="D32" s="21" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="E32" s="3" t="s">
         <v>52</v>
@@ -4034,16 +4031,16 @@
         <v>39</v>
       </c>
       <c r="K32" s="3" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="L32" s="3" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
       <c r="M32" s="28" t="s">
         <v>54</v>
       </c>
       <c r="N32" s="2" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="O32" s="5">
         <v>0.1</v>
@@ -4099,16 +4096,16 @@
         <v>2</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="D33" s="21" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="E33" s="3">
         <v>160</v>
       </c>
       <c r="F33" s="3" t="s">
-        <v>55</v>
+        <v>262</v>
       </c>
       <c r="G33" s="3"/>
       <c r="H33" s="3"/>
@@ -4119,17 +4116,15 @@
         <v>39</v>
       </c>
       <c r="K33" s="3" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="L33" s="3" t="s">
-        <v>56</v>
+        <v>260</v>
       </c>
       <c r="M33" s="28" t="s">
-        <v>57</v>
-      </c>
-      <c r="N33" s="2" t="s">
-        <v>200</v>
-      </c>
+        <v>261</v>
+      </c>
+      <c r="N33" s="2"/>
       <c r="O33" s="5">
         <v>0.27</v>
       </c>
@@ -4155,11 +4150,11 @@
       <c r="U33" s="4"/>
       <c r="V33" s="4" t="str">
         <f t="shared" si="19"/>
-        <v>4,160YCT-ND</v>
+        <v>4,10ZCT-ND</v>
       </c>
       <c r="W33" s="4" t="str">
         <f t="shared" si="6"/>
-        <v>2,160YCT-ND</v>
+        <v>2,10ZCT-ND</v>
       </c>
       <c r="X33" t="str">
         <f t="shared" si="24"/>
@@ -4167,11 +4162,11 @@
       </c>
       <c r="Y33" t="str">
         <f t="shared" si="8"/>
-        <v>594-5083NW160R0J|4</v>
+        <v/>
       </c>
       <c r="Z33" t="str">
         <f t="shared" si="9"/>
-        <v>FMP200FRF52-160R 4</v>
+        <v>FMP200JR-52-10R 4</v>
       </c>
     </row>
     <row r="34" spans="1:26" ht="17" thickBot="1">
@@ -4222,38 +4217,38 @@
         <v>1</v>
       </c>
       <c r="C35" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="D35" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="E35" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="F35" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="D35" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="E35" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="F35" s="3" t="s">
-        <v>61</v>
-      </c>
       <c r="G35" s="3" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="H35" s="3"/>
       <c r="I35" s="3">
         <v>2</v>
       </c>
       <c r="J35" s="3" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="K35" s="3" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="L35" s="3" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="M35" s="28" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="N35" s="2" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="O35" s="5">
         <v>1.68</v>
@@ -4308,36 +4303,36 @@
         <v>1</v>
       </c>
       <c r="C36" s="4" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="D36" s="4" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="E36" s="3" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="F36" s="3" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="G36" s="3" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="H36" s="3"/>
       <c r="I36" s="3">
         <v>1</v>
       </c>
       <c r="J36" s="3" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="K36" s="3"/>
       <c r="L36" s="3" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="M36" s="28" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="N36" s="2" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="O36" s="6">
         <v>15.41</v>
@@ -4392,38 +4387,38 @@
         <v>1</v>
       </c>
       <c r="C37" s="11" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="D37" s="11" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="E37" s="12" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="F37" s="12" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="G37" s="3" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="H37" s="12"/>
       <c r="I37" s="12">
         <v>2</v>
       </c>
       <c r="J37" s="12" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="K37" s="12" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="L37" s="12" t="s">
+        <v>117</v>
+      </c>
+      <c r="M37" s="12" t="s">
         <v>120</v>
       </c>
-      <c r="M37" s="12" t="s">
-        <v>123</v>
-      </c>
       <c r="N37" s="12" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="O37" s="19">
         <v>2.92</v>
@@ -4477,38 +4472,38 @@
         <v>1</v>
       </c>
       <c r="C38" s="11" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="D38" s="11" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="E38" s="12" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="F38" s="3" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
       <c r="G38" s="3" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="H38" s="12"/>
       <c r="I38" s="12">
         <v>1</v>
       </c>
       <c r="J38" s="12" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="K38" s="25" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="L38" s="12" t="s">
+        <v>207</v>
+      </c>
+      <c r="M38" s="12" t="s">
+        <v>210</v>
+      </c>
+      <c r="N38" s="2" t="s">
         <v>211</v>
-      </c>
-      <c r="M38" s="12" t="s">
-        <v>214</v>
-      </c>
-      <c r="N38" s="2" t="s">
-        <v>215</v>
       </c>
       <c r="O38" s="6">
         <v>2.4</v>
@@ -4562,13 +4557,13 @@
         <v>2</v>
       </c>
       <c r="C39" s="11" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="D39" s="11" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="E39" s="12" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="F39" s="3"/>
       <c r="G39" s="3"/>
@@ -4576,16 +4571,16 @@
       <c r="I39" s="12"/>
       <c r="J39" s="12"/>
       <c r="K39" s="25" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="L39" s="12" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="M39" s="12" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="N39" s="2" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="O39" s="6">
         <v>0.5</v>
@@ -4674,10 +4669,10 @@
         <v>1</v>
       </c>
       <c r="C41" s="4" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="D41" s="4" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="E41" s="3"/>
       <c r="F41" s="3"/>
@@ -4687,17 +4682,17 @@
         <v>1</v>
       </c>
       <c r="J41" s="3" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="K41" s="3"/>
       <c r="L41" s="3" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="M41" s="12" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="N41" s="12" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="O41" s="6">
         <v>15.33</v>
@@ -4770,10 +4765,10 @@
       <c r="A43" s="15"/>
       <c r="B43" s="15"/>
       <c r="C43" s="4" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="D43" s="4" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="E43" s="3"/>
       <c r="F43" s="3"/>
@@ -4807,13 +4802,13 @@
       </c>
       <c r="B44" s="15"/>
       <c r="C44" s="4" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="D44" s="4" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="E44" s="3" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="F44" s="3"/>
       <c r="G44" s="3"/>
@@ -4822,11 +4817,11 @@
         <v>1</v>
       </c>
       <c r="J44" s="3" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="K44" s="3"/>
       <c r="L44" s="3" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="M44" s="12"/>
       <c r="N44" s="3"/>
@@ -4859,10 +4854,10 @@
       </c>
       <c r="B45" s="15"/>
       <c r="C45" s="4" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="D45" s="4" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="E45" s="3"/>
       <c r="F45" s="3"/>
@@ -4873,7 +4868,7 @@
       <c r="K45" s="3"/>
       <c r="L45" s="3"/>
       <c r="M45" s="12" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="N45" s="3"/>
       <c r="O45" s="3">
@@ -4885,7 +4880,7 @@
       <c r="S45" s="6"/>
       <c r="T45" s="6"/>
       <c r="U45" s="4" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
     </row>
     <row r="46" spans="1:26" ht="17" thickBot="1">
@@ -4901,12 +4896,12 @@
       <c r="J46" s="4"/>
       <c r="K46" s="8"/>
       <c r="L46" s="29" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="M46" s="30"/>
       <c r="N46" s="23"/>
       <c r="O46" s="1" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="P46" s="1"/>
       <c r="Q46" s="10">
@@ -4926,7 +4921,7 @@
         <v>82.16</v>
       </c>
       <c r="U46" s="9" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
     </row>
   </sheetData>
@@ -4937,18 +4932,17 @@
   <hyperlinks>
     <hyperlink ref="M6" r:id="rId1" display="478-1910-ND" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
     <hyperlink ref="M13" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
-    <hyperlink ref="M17" r:id="rId3" display="P7307-ND" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
-    <hyperlink ref="M26" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
-    <hyperlink ref="M30" r:id="rId5" display="985-1047-1-ND" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
-    <hyperlink ref="M31" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
-    <hyperlink ref="M36" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
-    <hyperlink ref="M3" r:id="rId8" display="478-1842-ND" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
-    <hyperlink ref="M7" r:id="rId9" display="445-5312-ND" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
-    <hyperlink ref="M8" r:id="rId10" display="399-4148-ND" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
-    <hyperlink ref="M32" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
+    <hyperlink ref="M26" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="M30" r:id="rId4" display="985-1047-1-ND" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="M31" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="M36" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="M3" r:id="rId7" display="478-1842-ND" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="M7" r:id="rId8" display="445-5312-ND" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink ref="M8" r:id="rId9" display="399-4148-ND" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
+    <hyperlink ref="M32" r:id="rId10" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
   </hyperlinks>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="27" orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <legacyDrawing r:id="rId12"/>
+  <legacyDrawing r:id="rId11"/>
 </worksheet>
 </file>
</xml_diff>